<commit_message>
tambahakan data validasi di format
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yefta\Desktop\transaksi-usaha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831C0325-DC42-401B-8E67-1432DBB0120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD051AE-0EDB-45DA-8BFD-A974CC97F3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="maret" sheetId="1" r:id="rId1"/>
+    <sheet name="deposit" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Tanggal</t>
   </si>
@@ -43,14 +44,64 @@
   </si>
   <si>
     <t>alt+H+O+I</t>
+  </si>
+  <si>
+    <t>Waktu</t>
+  </si>
+  <si>
+    <t>paskan kolom</t>
+  </si>
+  <si>
+    <t>ctrl+;</t>
+  </si>
+  <si>
+    <t>tanggal</t>
+  </si>
+  <si>
+    <t>ctrl+shift+;</t>
+  </si>
+  <si>
+    <t>waktu</t>
+  </si>
+  <si>
+    <t>Yefta</t>
+  </si>
+  <si>
+    <t>Jourgant</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Harga</t>
+  </si>
+  <si>
+    <t>Total Laba</t>
+  </si>
+  <si>
+    <t>Metode $</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,10 +123,45 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -84,10 +170,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,151 +497,737 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C96B9B0-DBCC-4414-A41F-7F539C74510D}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="H2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G51" xr:uid="{80E836B1-CA73-430F-A9BE-A69DBCB2D137}">
+      <formula1>"Tunai, Dana"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509D0149-539F-4799-B8B7-7D5398715352}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3">
+        <f>SUMIF($B$2:$B$26,F2,$C$2:$C$26)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="e">
+        <f>(G2/(SUM($G$2:$G$3)))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3">
+        <f>SUMIF($B$2:$B$26,F3,$C$2:$C$26)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="e">
+        <f>(G3/(SUM($G$2:$G$3)))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{A789F32E-CC67-4AB1-8F40-BB4C6A13BAF2}">
+      <formula1>"Yefta, Jourgant"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
laporan 9 maret - 4 transaksi
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D8D8B1-3721-4FD0-AE2A-DA1713D437C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAECA24-5CC1-4BD9-BC94-99098A6DF481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
   </bookViews>
   <sheets>
     <sheet name="maret" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Tanggal</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Yefta</t>
   </si>
   <si>
-    <t>Jourgant</t>
-  </si>
-  <si>
     <t>Nama</t>
   </si>
   <si>
@@ -82,10 +79,82 @@
     <t>Harga</t>
   </si>
   <si>
-    <t>Total Laba</t>
-  </si>
-  <si>
     <t>Metode $</t>
+  </si>
+  <si>
+    <t>Utang?</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>tri 10k</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Tunai</t>
+  </si>
+  <si>
+    <t>Temp Utang</t>
+  </si>
+  <si>
+    <t>Jourgent</t>
+  </si>
+  <si>
+    <t>Hutang</t>
+  </si>
+  <si>
+    <t>(Rp)</t>
+  </si>
+  <si>
+    <t>(orang)</t>
+  </si>
+  <si>
+    <t>Total Penghasilan</t>
+  </si>
+  <si>
+    <t>Kotor</t>
+  </si>
+  <si>
+    <t>Laba</t>
+  </si>
+  <si>
+    <t>&lt;-- jangan dirubah</t>
+  </si>
+  <si>
+    <t>tsel flash 500MB</t>
+  </si>
+  <si>
+    <t>Victor Senduk</t>
+  </si>
+  <si>
+    <t>indsat 12k</t>
+  </si>
+  <si>
+    <t>tri 15k</t>
+  </si>
+  <si>
+    <t>Nadira Purnomo</t>
+  </si>
+  <si>
+    <t>Saldo Ewallet</t>
+  </si>
+  <si>
+    <t>(Input manual)</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Total Modal</t>
+  </si>
+  <si>
+    <t>error=(pndptn_bersih+saldo_sisa)-ttl_modal</t>
+  </si>
+  <si>
+    <t>^saldo sisa</t>
   </si>
 </sst>
 </file>
@@ -109,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,8 +191,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -147,9 +222,35 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -162,26 +263,90 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -189,6 +354,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -497,26 +667,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C96B9B0-DBCC-4414-A41F-7F539C74510D}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -527,7 +706,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -536,485 +715,892 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="J1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45359</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="3">
+        <v>12075</v>
+      </c>
+      <c r="E2" s="3">
+        <v>14000</v>
+      </c>
+      <c r="F2" s="3">
+        <f>SUM(E2)-SUM(D2)</f>
+        <v>1925</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I2" s="3"/>
-      <c r="L2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="L3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="L4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="18"/>
+      <c r="P2" s="17"/>
+      <c r="R2" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45360</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10450</v>
+      </c>
+      <c r="E3" s="3">
+        <v>12000</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F51" si="0">SUM(E3)-SUM(D3)</f>
+        <v>1550</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3">
+        <f>SUM($E$2:E51)</f>
+        <v>55000</v>
+      </c>
+      <c r="K3" s="14">
+        <f>SUM($F$2:F51)</f>
+        <v>7525</v>
+      </c>
+      <c r="L3" s="3">
+        <f>COUNTIF(H2:H51,TRUE)</f>
+        <v>3</v>
+      </c>
+      <c r="M3" s="3">
+        <f>SUMIF($H$2:$H$26,R2,$E$2:$E$26)</f>
+        <v>41000</v>
+      </c>
+      <c r="N3" s="3">
+        <v>2525</v>
+      </c>
+      <c r="O3" s="3">
+        <f>deposit!G4</f>
+        <v>50000</v>
+      </c>
+      <c r="P3" s="3">
+        <f>((J3-K3)+N3)-O3</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45360</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.84861111111111109</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="E4" s="3">
+        <v>12000</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45360</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3">
+        <v>14950</v>
+      </c>
+      <c r="E5" s="3">
+        <v>17000</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="13"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="R6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="M7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="R8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="F36" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="F38" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="F43" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="F45" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="F46" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="F47" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="F48" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="F49" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="F50" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="F51" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <mergeCells count="5">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="O1:O2"/>
+  </mergeCells>
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G51" xr:uid="{80E836B1-CA73-430F-A9BE-A69DBCB2D137}">
-      <formula1>"Tunai, Dana"</formula1>
+      <formula1>"Tunai, Gopay, Dana"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H51" xr:uid="{72FE33D0-D55F-4CC1-81A9-B97F7B497039}">
+      <formula1>"false, true"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1026,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509D0149-539F-4799-B8B7-7D5398715352}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,17 +1627,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1087,7 +1673,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3">
         <f>SUMIF($B$2:$B$26,F3,$C$2:$C$26)</f>
@@ -1108,6 +1694,13 @@
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3">
+        <f>G2+G3</f>
+        <v>50000</v>
+      </c>
       <c r="K4" t="s">
         <v>10</v>
       </c>
@@ -1226,12 +1819,13 @@
       <c r="C26" s="3"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{A789F32E-CC67-4AB1-8F40-BB4C6A13BAF2}">
-      <formula1>"Yefta, Jourgant"</formula1>
+      <formula1>"Yefta, Jourgent"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
10 maret 24 - 15:40
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAECA24-5CC1-4BD9-BC94-99098A6DF481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F153AA14-10F5-46AE-91F3-A96BA27CA16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
   </bookViews>
   <sheets>
-    <sheet name="maret" sheetId="1" r:id="rId1"/>
-    <sheet name="deposit" sheetId="2" r:id="rId2"/>
+    <sheet name="transaksi" sheetId="1" r:id="rId1"/>
+    <sheet name="wallet" sheetId="3" r:id="rId2"/>
+    <sheet name="deposit" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Tanggal</t>
   </si>
@@ -139,9 +140,6 @@
     <t>Nadira Purnomo</t>
   </si>
   <si>
-    <t>Saldo Ewallet</t>
-  </si>
-  <si>
     <t>(Input manual)</t>
   </si>
   <si>
@@ -155,6 +153,39 @@
   </si>
   <si>
     <t>^saldo sisa</t>
+  </si>
+  <si>
+    <t>indsat 5k</t>
+  </si>
+  <si>
+    <t>Dana</t>
+  </si>
+  <si>
+    <t>tsel 5k</t>
+  </si>
+  <si>
+    <t>Ovo</t>
+  </si>
+  <si>
+    <t>BNI</t>
+  </si>
+  <si>
+    <t>tip</t>
+  </si>
+  <si>
+    <t>total uang</t>
+  </si>
+  <si>
+    <t>hutang-Tunai</t>
+  </si>
+  <si>
+    <t>Ditangan</t>
+  </si>
+  <si>
+    <t>Gopay</t>
+  </si>
+  <si>
+    <t>Total Uang Ditangan (Kotor)</t>
   </si>
 </sst>
 </file>
@@ -178,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,8 +228,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -306,25 +349,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,8 +390,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -346,6 +397,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -667,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C96B9B0-DBCC-4414-A41F-7F539C74510D}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:S201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +780,7 @@
     <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.21875" bestFit="1" customWidth="1"/>
@@ -723,24 +814,24 @@
       <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="10" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" s="16" t="s">
+      <c r="M1" s="12"/>
+      <c r="N1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="P1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -771,23 +862,23 @@
         <v>0</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="18"/>
-      <c r="P2" s="17"/>
+      <c r="N2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="17"/>
+      <c r="P2" s="16"/>
       <c r="R2" s="3" t="b">
         <v>1</v>
       </c>
@@ -809,7 +900,7 @@
         <v>12000</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F51" si="0">SUM(E3)-SUM(D3)</f>
+        <f t="shared" ref="F3:F53" si="0">SUM(E3)-SUM(D3)</f>
         <v>1550</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -823,11 +914,11 @@
       </c>
       <c r="J3" s="3">
         <f>SUM($E$2:E51)</f>
-        <v>55000</v>
-      </c>
-      <c r="K3" s="14">
+        <v>105000</v>
+      </c>
+      <c r="K3" s="8">
         <f>SUM($F$2:F51)</f>
-        <v>7525</v>
+        <v>17725</v>
       </c>
       <c r="L3" s="3">
         <f>COUNTIF(H2:H51,TRUE)</f>
@@ -838,11 +929,11 @@
         <v>41000</v>
       </c>
       <c r="N3" s="3">
-        <v>2525</v>
+        <v>12725</v>
       </c>
       <c r="O3" s="3">
         <f>deposit!G4</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="P3" s="3">
         <f>((J3-K3)+N3)-O3</f>
@@ -885,7 +976,7 @@
         <v>33</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -917,23 +1008,37 @@
       <c r="I5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="13"/>
+      <c r="S5" s="14"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5850</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7000</v>
+      </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+        <v>1150</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="R6" s="3" t="s">
         <v>5</v>
@@ -943,21 +1048,32 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5850</v>
+      </c>
+      <c r="E7" s="3">
+        <v>7000</v>
+      </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+        <v>1150</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I7" s="3"/>
-      <c r="M7" t="s">
-        <v>41</v>
-      </c>
       <c r="R7" s="3" t="s">
         <v>8</v>
       </c>
@@ -966,17 +1082,31 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.61527777777777781</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5275</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7000</v>
+      </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+        <v>1725</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="R8" s="3" t="s">
         <v>10</v>
@@ -986,73 +1116,144 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5850</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7000</v>
+      </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+        <v>1150</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5850</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7000</v>
+      </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+        <v>1150</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I10" s="3"/>
+      <c r="R10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5275</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7000</v>
+      </c>
       <c r="F11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+        <v>1725</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5850</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7000</v>
+      </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+        <v>1150</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="A13" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.63402777777777775</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>1000</v>
+      </c>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+        <v>1000</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1586,6 +1787,2106 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <f t="shared" ref="F52:F54" si="1">SUM(E52)-SUM(D52)</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3">
+        <f t="shared" ref="F55:F118" si="2">SUM(E55)-SUM(D55)</f>
+        <v>0</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="3"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="3"/>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="3"/>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="3"/>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="3"/>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="3"/>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+      <c r="I113" s="3"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114" s="3"/>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G114" s="3"/>
+      <c r="H114" s="3"/>
+      <c r="I114" s="3"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" s="3"/>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116" s="3"/>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
+      <c r="I116" s="3"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" s="3"/>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+      <c r="I117" s="3"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" s="3"/>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119" s="3"/>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3">
+        <f t="shared" ref="F119:F182" si="3">SUM(E119)-SUM(D119)</f>
+        <v>0</v>
+      </c>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3"/>
+      <c r="I119" s="3"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" s="3"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G120" s="3"/>
+      <c r="H120" s="3"/>
+      <c r="I120" s="3"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" s="3"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" s="3"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3"/>
+      <c r="I122" s="3"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" s="3"/>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G123" s="3"/>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" s="3"/>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G124" s="3"/>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" s="3"/>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G125" s="3"/>
+      <c r="H125" s="3"/>
+      <c r="I125" s="3"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G127" s="3"/>
+      <c r="H127" s="3"/>
+      <c r="I127" s="3"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" s="3"/>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G128" s="3"/>
+      <c r="H128" s="3"/>
+      <c r="I128" s="3"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" s="3"/>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G130" s="3"/>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G131" s="3"/>
+      <c r="H131" s="3"/>
+      <c r="I131" s="3"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G132" s="3"/>
+      <c r="H132" s="3"/>
+      <c r="I132" s="3"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" s="3"/>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G133" s="3"/>
+      <c r="H133" s="3"/>
+      <c r="I133" s="3"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G134" s="3"/>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G135" s="3"/>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G136" s="3"/>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A137" s="3"/>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138" s="3"/>
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G138" s="3"/>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+      <c r="E139" s="3"/>
+      <c r="F139" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G139" s="3"/>
+      <c r="H139" s="3"/>
+      <c r="I139" s="3"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G140" s="3"/>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G141" s="3"/>
+      <c r="H141" s="3"/>
+      <c r="I141" s="3"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G142" s="3"/>
+      <c r="H142" s="3"/>
+      <c r="I142" s="3"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+      <c r="E143" s="3"/>
+      <c r="F143" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G143" s="3"/>
+      <c r="H143" s="3"/>
+      <c r="I143" s="3"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G144" s="3"/>
+      <c r="H144" s="3"/>
+      <c r="I144" s="3"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A145" s="3"/>
+      <c r="B145" s="3"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G145" s="3"/>
+      <c r="H145" s="3"/>
+      <c r="I145" s="3"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" s="3"/>
+      <c r="B146" s="3"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G146" s="3"/>
+      <c r="H146" s="3"/>
+      <c r="I146" s="3"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147" s="3"/>
+      <c r="B147" s="3"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3"/>
+      <c r="E147" s="3"/>
+      <c r="F147" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G147" s="3"/>
+      <c r="H147" s="3"/>
+      <c r="I147" s="3"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G149" s="3"/>
+      <c r="H149" s="3"/>
+      <c r="I149" s="3"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A150" s="3"/>
+      <c r="B150" s="3"/>
+      <c r="C150" s="3"/>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G150" s="3"/>
+      <c r="H150" s="3"/>
+      <c r="I150" s="3"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A151" s="3"/>
+      <c r="B151" s="3"/>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G151" s="3"/>
+      <c r="H151" s="3"/>
+      <c r="I151" s="3"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A152" s="3"/>
+      <c r="B152" s="3"/>
+      <c r="C152" s="3"/>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G152" s="3"/>
+      <c r="H152" s="3"/>
+      <c r="I152" s="3"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A153" s="3"/>
+      <c r="B153" s="3"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
+      <c r="E153" s="3"/>
+      <c r="F153" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G153" s="3"/>
+      <c r="H153" s="3"/>
+      <c r="I153" s="3"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G154" s="3"/>
+      <c r="H154" s="3"/>
+      <c r="I154" s="3"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G155" s="3"/>
+      <c r="H155" s="3"/>
+      <c r="I155" s="3"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3"/>
+      <c r="E156" s="3"/>
+      <c r="F156" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G156" s="3"/>
+      <c r="H156" s="3"/>
+      <c r="I156" s="3"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A157" s="3"/>
+      <c r="B157" s="3"/>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G157" s="3"/>
+      <c r="H157" s="3"/>
+      <c r="I157" s="3"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A158" s="3"/>
+      <c r="B158" s="3"/>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G158" s="3"/>
+      <c r="H158" s="3"/>
+      <c r="I158" s="3"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A159" s="3"/>
+      <c r="B159" s="3"/>
+      <c r="C159" s="3"/>
+      <c r="D159" s="3"/>
+      <c r="E159" s="3"/>
+      <c r="F159" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G159" s="3"/>
+      <c r="H159" s="3"/>
+      <c r="I159" s="3"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160" s="3"/>
+      <c r="B160" s="3"/>
+      <c r="C160" s="3"/>
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G160" s="3"/>
+      <c r="H160" s="3"/>
+      <c r="I160" s="3"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A161" s="3"/>
+      <c r="B161" s="3"/>
+      <c r="C161" s="3"/>
+      <c r="D161" s="3"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G161" s="3"/>
+      <c r="H161" s="3"/>
+      <c r="I161" s="3"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162" s="3"/>
+      <c r="B162" s="3"/>
+      <c r="C162" s="3"/>
+      <c r="D162" s="3"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G162" s="3"/>
+      <c r="H162" s="3"/>
+      <c r="I162" s="3"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A163" s="3"/>
+      <c r="B163" s="3"/>
+      <c r="C163" s="3"/>
+      <c r="D163" s="3"/>
+      <c r="E163" s="3"/>
+      <c r="F163" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G163" s="3"/>
+      <c r="H163" s="3"/>
+      <c r="I163" s="3"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A164" s="3"/>
+      <c r="B164" s="3"/>
+      <c r="C164" s="3"/>
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G164" s="3"/>
+      <c r="H164" s="3"/>
+      <c r="I164" s="3"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G165" s="3"/>
+      <c r="H165" s="3"/>
+      <c r="I165" s="3"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A166" s="3"/>
+      <c r="B166" s="3"/>
+      <c r="C166" s="3"/>
+      <c r="D166" s="3"/>
+      <c r="E166" s="3"/>
+      <c r="F166" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G166" s="3"/>
+      <c r="H166" s="3"/>
+      <c r="I166" s="3"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A167" s="3"/>
+      <c r="B167" s="3"/>
+      <c r="C167" s="3"/>
+      <c r="D167" s="3"/>
+      <c r="E167" s="3"/>
+      <c r="F167" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G167" s="3"/>
+      <c r="H167" s="3"/>
+      <c r="I167" s="3"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A168" s="3"/>
+      <c r="B168" s="3"/>
+      <c r="C168" s="3"/>
+      <c r="D168" s="3"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G168" s="3"/>
+      <c r="H168" s="3"/>
+      <c r="I168" s="3"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A169" s="3"/>
+      <c r="B169" s="3"/>
+      <c r="C169" s="3"/>
+      <c r="D169" s="3"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G169" s="3"/>
+      <c r="H169" s="3"/>
+      <c r="I169" s="3"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A170" s="3"/>
+      <c r="B170" s="3"/>
+      <c r="C170" s="3"/>
+      <c r="D170" s="3"/>
+      <c r="E170" s="3"/>
+      <c r="F170" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G170" s="3"/>
+      <c r="H170" s="3"/>
+      <c r="I170" s="3"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A171" s="3"/>
+      <c r="B171" s="3"/>
+      <c r="C171" s="3"/>
+      <c r="D171" s="3"/>
+      <c r="E171" s="3"/>
+      <c r="F171" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G171" s="3"/>
+      <c r="H171" s="3"/>
+      <c r="I171" s="3"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A172" s="3"/>
+      <c r="B172" s="3"/>
+      <c r="C172" s="3"/>
+      <c r="D172" s="3"/>
+      <c r="E172" s="3"/>
+      <c r="F172" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G172" s="3"/>
+      <c r="H172" s="3"/>
+      <c r="I172" s="3"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A173" s="3"/>
+      <c r="B173" s="3"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="3"/>
+      <c r="E173" s="3"/>
+      <c r="F173" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G173" s="3"/>
+      <c r="H173" s="3"/>
+      <c r="I173" s="3"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A174" s="3"/>
+      <c r="B174" s="3"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="3"/>
+      <c r="E174" s="3"/>
+      <c r="F174" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G174" s="3"/>
+      <c r="H174" s="3"/>
+      <c r="I174" s="3"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A175" s="3"/>
+      <c r="B175" s="3"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="3"/>
+      <c r="E175" s="3"/>
+      <c r="F175" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G175" s="3"/>
+      <c r="H175" s="3"/>
+      <c r="I175" s="3"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A176" s="3"/>
+      <c r="B176" s="3"/>
+      <c r="C176" s="3"/>
+      <c r="D176" s="3"/>
+      <c r="E176" s="3"/>
+      <c r="F176" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G176" s="3"/>
+      <c r="H176" s="3"/>
+      <c r="I176" s="3"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A177" s="3"/>
+      <c r="B177" s="3"/>
+      <c r="C177" s="3"/>
+      <c r="D177" s="3"/>
+      <c r="E177" s="3"/>
+      <c r="F177" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G177" s="3"/>
+      <c r="H177" s="3"/>
+      <c r="I177" s="3"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A178" s="3"/>
+      <c r="B178" s="3"/>
+      <c r="C178" s="3"/>
+      <c r="D178" s="3"/>
+      <c r="E178" s="3"/>
+      <c r="F178" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G178" s="3"/>
+      <c r="H178" s="3"/>
+      <c r="I178" s="3"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A179" s="3"/>
+      <c r="B179" s="3"/>
+      <c r="C179" s="3"/>
+      <c r="D179" s="3"/>
+      <c r="E179" s="3"/>
+      <c r="F179" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G179" s="3"/>
+      <c r="H179" s="3"/>
+      <c r="I179" s="3"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A180" s="3"/>
+      <c r="B180" s="3"/>
+      <c r="C180" s="3"/>
+      <c r="D180" s="3"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G180" s="3"/>
+      <c r="H180" s="3"/>
+      <c r="I180" s="3"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A181" s="3"/>
+      <c r="B181" s="3"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="3"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G181" s="3"/>
+      <c r="H181" s="3"/>
+      <c r="I181" s="3"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A182" s="3"/>
+      <c r="B182" s="3"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G182" s="3"/>
+      <c r="H182" s="3"/>
+      <c r="I182" s="3"/>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A183" s="3"/>
+      <c r="B183" s="3"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="3"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="3">
+        <f t="shared" ref="F183:F201" si="4">SUM(E183)-SUM(D183)</f>
+        <v>0</v>
+      </c>
+      <c r="G183" s="3"/>
+      <c r="H183" s="3"/>
+      <c r="I183" s="3"/>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A184" s="3"/>
+      <c r="B184" s="3"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="3"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G184" s="3"/>
+      <c r="H184" s="3"/>
+      <c r="I184" s="3"/>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A185" s="3"/>
+      <c r="B185" s="3"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="3"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G185" s="3"/>
+      <c r="H185" s="3"/>
+      <c r="I185" s="3"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A186" s="3"/>
+      <c r="B186" s="3"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="3"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G186" s="3"/>
+      <c r="H186" s="3"/>
+      <c r="I186" s="3"/>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A187" s="3"/>
+      <c r="B187" s="3"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="3"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G187" s="3"/>
+      <c r="H187" s="3"/>
+      <c r="I187" s="3"/>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A188" s="3"/>
+      <c r="B188" s="3"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="3"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G188" s="3"/>
+      <c r="H188" s="3"/>
+      <c r="I188" s="3"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A189" s="3"/>
+      <c r="B189" s="3"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="3"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G189" s="3"/>
+      <c r="H189" s="3"/>
+      <c r="I189" s="3"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A190" s="3"/>
+      <c r="B190" s="3"/>
+      <c r="C190" s="3"/>
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G190" s="3"/>
+      <c r="H190" s="3"/>
+      <c r="I190" s="3"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A191" s="3"/>
+      <c r="B191" s="3"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="3"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G191" s="3"/>
+      <c r="H191" s="3"/>
+      <c r="I191" s="3"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A192" s="3"/>
+      <c r="B192" s="3"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G192" s="3"/>
+      <c r="H192" s="3"/>
+      <c r="I192" s="3"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A193" s="3"/>
+      <c r="B193" s="3"/>
+      <c r="C193" s="3"/>
+      <c r="D193" s="3"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G193" s="3"/>
+      <c r="H193" s="3"/>
+      <c r="I193" s="3"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A194" s="3"/>
+      <c r="B194" s="3"/>
+      <c r="C194" s="3"/>
+      <c r="D194" s="3"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G194" s="3"/>
+      <c r="H194" s="3"/>
+      <c r="I194" s="3"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A195" s="3"/>
+      <c r="B195" s="3"/>
+      <c r="C195" s="3"/>
+      <c r="D195" s="3"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G195" s="3"/>
+      <c r="H195" s="3"/>
+      <c r="I195" s="3"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A196" s="3"/>
+      <c r="B196" s="3"/>
+      <c r="C196" s="3"/>
+      <c r="D196" s="3"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G196" s="3"/>
+      <c r="H196" s="3"/>
+      <c r="I196" s="3"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A197" s="3"/>
+      <c r="B197" s="3"/>
+      <c r="C197" s="3"/>
+      <c r="D197" s="3"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G197" s="3"/>
+      <c r="H197" s="3"/>
+      <c r="I197" s="3"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A198" s="3"/>
+      <c r="B198" s="3"/>
+      <c r="C198" s="3"/>
+      <c r="D198" s="3"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G198" s="3"/>
+      <c r="H198" s="3"/>
+      <c r="I198" s="3"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A199" s="3"/>
+      <c r="B199" s="3"/>
+      <c r="C199" s="3"/>
+      <c r="D199" s="3"/>
+      <c r="E199" s="3"/>
+      <c r="F199" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G199" s="3"/>
+      <c r="H199" s="3"/>
+      <c r="I199" s="3"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A200" s="3"/>
+      <c r="B200" s="3"/>
+      <c r="C200" s="3"/>
+      <c r="D200" s="3"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G200" s="3"/>
+      <c r="H200" s="3"/>
+      <c r="I200" s="3"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A201" s="3"/>
+      <c r="B201" s="3"/>
+      <c r="C201" s="3"/>
+      <c r="D201" s="3"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G201" s="3"/>
+      <c r="H201" s="3"/>
+      <c r="I201" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1596,10 +3897,10 @@
     <mergeCell ref="O1:O2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G51" xr:uid="{80E836B1-CA73-430F-A9BE-A69DBCB2D137}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G201" xr:uid="{80E836B1-CA73-430F-A9BE-A69DBCB2D137}">
       <formula1>"Tunai, Gopay, Dana"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H51" xr:uid="{72FE33D0-D55F-4CC1-81A9-B97F7B497039}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H201" xr:uid="{72FE33D0-D55F-4CC1-81A9-B97F7B497039}">
       <formula1>"false, true"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1609,11 +3910,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3E639-FBD1-4498-B33D-4B47BAF93CDC}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>transaksi!M3</f>
+        <v>41000</v>
+      </c>
+      <c r="B3" s="28">
+        <v>14000</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="26">
+        <f>B3+A3</f>
+        <v>55000</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="31">
+        <v>50000</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31">
+        <v>12725</v>
+      </c>
+      <c r="G4" s="29">
+        <f>SUM($A$4:$F$4)</f>
+        <v>117725</v>
+      </c>
+      <c r="H4" s="30">
+        <f>G4-$A$3</f>
+        <v>76725</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509D0149-539F-4799-B8B7-7D5398715352}">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,11 +4033,11 @@
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1655,7 +4056,7 @@
       </c>
       <c r="G2" s="3">
         <f>SUMIF($B$2:$B$26,F2,$C$2:$C$26)</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="H2" s="3">
         <f>(G2/(SUM($G$2:$G$3)))*100</f>
@@ -1669,9 +4070,15 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>50000</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1699,7 +4106,7 @@
       </c>
       <c r="G4" s="3">
         <f>G2+G3</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
11 maret 24 - 11:00
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3B3BD1-A910-433B-9AA9-54C45CEDB079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AD0618-6F4F-4A2F-8C2A-31A18F55E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
   <si>
     <t>Tanggal</t>
   </si>
@@ -195,6 +195,39 @@
   </si>
   <si>
     <t>&lt;- ada yg salah</t>
+  </si>
+  <si>
+    <t>^ubah ini setiap transaksi</t>
+  </si>
+  <si>
+    <t>tsel flash 4GB</t>
+  </si>
+  <si>
+    <t>om tris - trangkil</t>
+  </si>
+  <si>
+    <t>pln pasca</t>
+  </si>
+  <si>
+    <t>pln token</t>
+  </si>
+  <si>
+    <t>tsel 50k</t>
+  </si>
+  <si>
+    <t>ma titin</t>
+  </si>
+  <si>
+    <t>tri 3GB/3hri</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>^^</t>
+  </si>
+  <si>
+    <t>tidak termasuk biaya admin perpindahan dana antar bank</t>
   </si>
 </sst>
 </file>
@@ -453,7 +486,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -468,10 +501,61 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFFF9999"/>
       <color rgb="FFFF0000"/>
       <color rgb="FFFF3300"/>
       <color rgb="FF66FF66"/>
@@ -787,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C96B9B0-DBCC-4414-A41F-7F539C74510D}">
   <dimension ref="A1:AA201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,14 +888,14 @@
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="54" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="1.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -946,31 +1030,31 @@
       </c>
       <c r="J3" s="3">
         <f>SUM($E$2:E201)</f>
-        <v>105000</v>
+        <v>432000</v>
       </c>
       <c r="K3" s="7">
         <f>SUM($F$2:F201)</f>
-        <v>17725</v>
+        <v>34367</v>
       </c>
       <c r="L3" s="3">
         <f>COUNTIF(H2:H201,TRUE)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M3" s="3">
         <f>SUMIF($H$2:$H$201,TRUE,$E$2:$E$201)</f>
-        <v>41000</v>
+        <v>200000</v>
       </c>
       <c r="N3" s="3">
         <f>wallet!G4</f>
-        <v>117725</v>
+        <v>354367</v>
       </c>
       <c r="O3" s="3">
         <f>deposit!G4</f>
-        <v>100000</v>
+        <v>320000</v>
       </c>
       <c r="P3" s="3">
         <f>SUM($D$2:$D$201)</f>
-        <v>87275</v>
+        <v>397633</v>
       </c>
       <c r="Q3" s="3" t="b">
         <f>((O3-P3)+J3) &lt;&gt; N3</f>
@@ -1291,116 +1375,240 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="A14" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.77986111111111112</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3">
+        <v>10450</v>
+      </c>
+      <c r="E14" s="3">
+        <v>12000</v>
+      </c>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+        <v>1550</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="3">
+        <v>58100</v>
+      </c>
+      <c r="E15" s="3">
+        <v>62000</v>
+      </c>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+        <v>3900</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="A16" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.37083333333333335</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="3">
+        <v>29308</v>
+      </c>
+      <c r="E16" s="3">
+        <v>31000</v>
+      </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+        <v>1692</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="A17" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.38263888888888886</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="3">
+        <v>50500</v>
+      </c>
+      <c r="E17" s="3">
+        <v>52000</v>
+      </c>
       <c r="F17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+        <v>1500</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="A18" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="3">
+        <v>49750</v>
+      </c>
+      <c r="E18" s="3">
+        <v>52000</v>
+      </c>
       <c r="F18" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+        <v>2250</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.39513888888888887</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3">
+        <v>12750</v>
+      </c>
+      <c r="E19" s="3">
+        <v>14000</v>
+      </c>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+        <v>1250</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.40277777777777779</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="3">
+        <v>49750</v>
+      </c>
+      <c r="E20" s="3">
+        <v>52000</v>
+      </c>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+        <v>2250</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.41458333333333336</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="3">
+        <v>49750</v>
+      </c>
+      <c r="E21" s="3">
+        <v>52000</v>
+      </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+        <v>2250</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
@@ -3933,18 +4141,18 @@
     <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <conditionalFormatting sqref="M3">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>$M$3 &gt; 50000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$Q$3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G201" xr:uid="{80E836B1-CA73-430F-A9BE-A69DBCB2D137}">
-      <formula1>"Tunai, Gopay, Dana"</formula1>
+      <formula1>"Tunai, Gopay, Dana, Ovo, BNI"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H201" xr:uid="{72FE33D0-D55F-4CC1-81A9-B97F7B497039}">
       <formula1>"false, true"</formula1>
@@ -3957,15 +4165,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3E639-FBD1-4498-B33D-4B47BAF93CDC}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>45</v>
       </c>
@@ -3981,7 +4189,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>42</v>
       </c>
@@ -4001,13 +4209,13 @@
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>transaksi!M3</f>
-        <v>41000</v>
+        <v>200000</v>
       </c>
       <c r="B3" s="9">
-        <v>14000</v>
+        <v>66000</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4016,27 +4224,45 @@
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="24">
         <f>B3+A3</f>
-        <v>55000</v>
+        <v>266000</v>
       </c>
       <c r="B4" s="25"/>
-      <c r="C4" s="12">
-        <v>50000</v>
-      </c>
+      <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12">
-        <v>12725</v>
+        <v>88367</v>
       </c>
       <c r="G4" s="10">
         <f>SUM($A$4:$F$4)</f>
-        <v>117725</v>
+        <v>354367</v>
       </c>
       <c r="H4" s="11">
         <f>G4-$A$3</f>
-        <v>76725</v>
+        <v>154367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4060,7 +4286,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4115,11 +4341,11 @@
       </c>
       <c r="G2" s="3">
         <f>SUMIF($B$2:$B$26,F2,$E$2:$E$26)</f>
-        <v>100000</v>
+        <v>270000</v>
       </c>
       <c r="H2" s="3">
         <f>(G2/(SUM($G$2:$G$3)))*100</f>
-        <v>100</v>
+        <v>84.375</v>
       </c>
       <c r="K2" t="s">
         <v>4</v>
@@ -4150,11 +4376,11 @@
       </c>
       <c r="G3" s="3">
         <f>SUMIF($B$2:$B$26,F3,$E$2:$E$26)</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="H3" s="3">
         <f>(G3/(SUM($G$2:$G$3)))*100</f>
-        <v>0</v>
+        <v>15.625</v>
       </c>
       <c r="K3" t="s">
         <v>7</v>
@@ -4164,17 +4390,28 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13">
+        <v>171000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>170000</v>
+      </c>
       <c r="F4" s="15" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="3">
         <f>G2+G3</f>
-        <v>100000</v>
+        <v>320000</v>
       </c>
       <c r="K4" t="s">
         <v>9</v>
@@ -4184,13 +4421,21 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="13">
+        <v>51000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1000</v>
+      </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
11 maret 24 - 20:26
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AD0618-6F4F-4A2F-8C2A-31A18F55E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E031BA-831F-4568-81A2-643A63A01668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
+    <workbookView xWindow="0" yWindow="324" windowWidth="12192" windowHeight="10236" activeTab="2" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
   </bookViews>
   <sheets>
     <sheet name="transaksi" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="69">
   <si>
     <t>Tanggal</t>
   </si>
@@ -104,9 +104,6 @@
     <t>(Rp)</t>
   </si>
   <si>
-    <t>(orang)</t>
-  </si>
-  <si>
     <t>Total Penghasilan</t>
   </si>
   <si>
@@ -228,6 +225,15 @@
   </si>
   <si>
     <t>tidak termasuk biaya admin perpindahan dana antar bank</t>
+  </si>
+  <si>
+    <t>tsel inter sakti in-app</t>
+  </si>
+  <si>
+    <t>trnsksi</t>
+  </si>
+  <si>
+    <t>Pembagian Hasil (Rp)</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -482,11 +488,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -498,55 +505,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -871,15 +829,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C96B9B0-DBCC-4414-A41F-7F539C74510D}">
   <dimension ref="A1:AA201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
@@ -892,7 +850,7 @@
     <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="54" bestFit="1" customWidth="1"/>
@@ -929,7 +887,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" s="17"/>
       <c r="L1" s="16" t="s">
@@ -937,22 +895,22 @@
       </c>
       <c r="M1" s="17"/>
       <c r="N1" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" t="s">
         <v>48</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>49</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
@@ -963,7 +921,7 @@
         <v>0.97916666666666663</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3">
         <v>12075</v>
@@ -983,13 +941,13 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>24</v>
@@ -1030,11 +988,11 @@
       </c>
       <c r="J3" s="3">
         <f>SUM($E$2:E201)</f>
-        <v>432000</v>
+        <v>457000</v>
       </c>
       <c r="K3" s="7">
         <f>SUM($F$2:F201)</f>
-        <v>34367</v>
+        <v>36367</v>
       </c>
       <c r="L3" s="3">
         <f>COUNTIF(H2:H201,TRUE)</f>
@@ -1046,7 +1004,7 @@
       </c>
       <c r="N3" s="3">
         <f>wallet!G4</f>
-        <v>354367</v>
+        <v>356367</v>
       </c>
       <c r="O3" s="3">
         <f>deposit!G4</f>
@@ -1054,17 +1012,17 @@
       </c>
       <c r="P3" s="3">
         <f>SUM($D$2:$D$201)</f>
-        <v>397633</v>
+        <v>420633</v>
       </c>
       <c r="Q3" s="3" t="b">
         <f>((O3-P3)+J3) &lt;&gt; N3</f>
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
@@ -1075,7 +1033,7 @@
         <v>0.84861111111111109</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3">
         <v>10000</v>
@@ -1094,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
@@ -1105,7 +1063,7 @@
         <v>0.87152777777777779</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3">
         <v>14950</v>
@@ -1124,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T5" s="18" t="s">
         <v>20</v>
@@ -1140,7 +1098,7 @@
         <v>0.61250000000000004</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3">
         <v>5850</v>
@@ -1153,7 +1111,7 @@
         <v>1150</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="3" t="b">
         <v>0</v>
@@ -1175,7 +1133,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3">
         <v>5850</v>
@@ -1188,7 +1146,7 @@
         <v>1150</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" s="3" t="b">
         <v>0</v>
@@ -1210,7 +1168,7 @@
         <v>0.61527777777777781</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="3">
         <v>5275</v>
@@ -1223,7 +1181,7 @@
         <v>1725</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="3" t="b">
         <v>0</v>
@@ -1244,7 +1202,7 @@
         <v>0.6166666666666667</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3">
         <v>5850</v>
@@ -1257,7 +1215,7 @@
         <v>1150</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" s="3" t="b">
         <v>0</v>
@@ -1272,7 +1230,7 @@
         <v>0.6166666666666667</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="3">
         <v>5850</v>
@@ -1285,7 +1243,7 @@
         <v>1150</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="3" t="b">
         <v>0</v>
@@ -1300,7 +1258,7 @@
         <v>0.61736111111111114</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="3">
         <v>5275</v>
@@ -1313,7 +1271,7 @@
         <v>1725</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="3" t="b">
         <v>0</v>
@@ -1328,7 +1286,7 @@
         <v>0.61736111111111114</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3">
         <v>5850</v>
@@ -1341,7 +1299,7 @@
         <v>1150</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="3" t="b">
         <v>0</v>
@@ -1356,7 +1314,7 @@
         <v>0.63402777777777775</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3">
@@ -1367,7 +1325,7 @@
         <v>1000</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13" s="3" t="b">
         <v>0</v>
@@ -1395,7 +1353,7 @@
         <v>1550</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="3" t="b">
         <v>0</v>
@@ -1410,7 +1368,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3">
         <v>58100</v>
@@ -1429,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
@@ -1440,7 +1398,7 @@
         <v>0.37083333333333335</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="3">
         <v>29308</v>
@@ -1459,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1470,7 +1428,7 @@
         <v>0.38263888888888886</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="3">
         <v>50500</v>
@@ -1498,7 +1456,7 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="3">
         <v>49750</v>
@@ -1517,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1528,7 +1486,7 @@
         <v>0.39513888888888887</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3">
         <v>12750</v>
@@ -1558,7 +1516,7 @@
         <v>0.40277777777777779</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="3">
         <v>49750</v>
@@ -1577,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1588,7 +1546,7 @@
         <v>0.41458333333333336</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="3">
         <v>49750</v>
@@ -1607,21 +1565,35 @@
         <v>1</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.50486111111111109</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="3">
+        <v>23000</v>
+      </c>
+      <c r="E22" s="3">
+        <v>25000</v>
+      </c>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+        <v>2000</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -4168,14 +4140,14 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -4186,25 +4158,25 @@
         <v>13</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
@@ -4215,7 +4187,7 @@
         <v>200000</v>
       </c>
       <c r="B3" s="9">
-        <v>66000</v>
+        <v>91000</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4227,42 +4199,42 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="24">
         <f>B3+A3</f>
-        <v>266000</v>
+        <v>291000</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12">
-        <v>88367</v>
+        <v>65367</v>
       </c>
       <c r="G4" s="10">
         <f>SUM($A$4:$F$4)</f>
-        <v>354367</v>
+        <v>356367</v>
       </c>
       <c r="H4" s="11">
         <f>G4-$A$3</f>
-        <v>154367</v>
+        <v>156367</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
         <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4285,14 +4257,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509D0149-539F-4799-B8B7-7D5398715352}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -4303,13 +4283,13 @@
         <v>12</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>13</v>
@@ -4457,6 +4437,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F7" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -4467,8 +4451,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="33">
+        <f>(transaksi!$K$3)*(H2/100)</f>
+        <v>30684.65625</v>
+      </c>
       <c r="K8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -4480,6 +4471,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="33">
+        <f>(transaksi!$K$3)*(H3/100)</f>
+        <v>5682.34375</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
@@ -4653,8 +4651,9 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{A789F32E-CC67-4AB1-8F40-BB4C6A13BAF2}">

</xml_diff>

<commit_message>
memulai 12 maret 24
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E031BA-831F-4568-81A2-643A63A01668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27FA29D-8FB6-4518-AD1D-5455DA44924D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="324" windowWidth="12192" windowHeight="10236" activeTab="2" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B284D9F5-20DB-4035-B147-5B88DE1DC625}"/>
   </bookViews>
   <sheets>
     <sheet name="transaksi" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>Tanggal</t>
   </si>
@@ -437,6 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,7 +489,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,7 +830,7 @@
   <dimension ref="A1:AA201"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="A23" sqref="A23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,24 +886,24 @@
       <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="16" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="20" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="24" t="s">
         <v>47</v>
       </c>
       <c r="T1" t="s">
@@ -952,10 +952,10 @@
       <c r="M2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="23"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="24"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -988,23 +988,23 @@
       </c>
       <c r="J3" s="3">
         <f>SUM($E$2:E201)</f>
-        <v>457000</v>
+        <v>462000</v>
       </c>
       <c r="K3" s="7">
         <f>SUM($F$2:F201)</f>
-        <v>36367</v>
+        <v>41367</v>
       </c>
       <c r="L3" s="3">
         <f>COUNTIF(H2:H201,TRUE)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M3" s="3">
         <f>SUMIF($H$2:$H$201,TRUE,$E$2:$E$201)</f>
-        <v>200000</v>
+        <v>55000</v>
       </c>
       <c r="N3" s="3">
         <f>wallet!G4</f>
-        <v>356367</v>
+        <v>361367</v>
       </c>
       <c r="O3" s="3">
         <f>deposit!G4</f>
@@ -1084,10 +1084,10 @@
       <c r="I5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="T5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="U5" s="19"/>
+      <c r="U5" s="20"/>
       <c r="V5" s="8"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
@@ -1381,10 +1381,10 @@
         <v>3900</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H15" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>57</v>
@@ -1411,10 +1411,10 @@
         <v>1692</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H16" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>57</v>
@@ -1469,7 +1469,7 @@
         <v>2250</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H18" s="3" t="b">
         <v>0</v>
@@ -1529,7 +1529,7 @@
         <v>2250</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H20" s="3" t="b">
         <v>0</v>
@@ -1559,10 +1559,10 @@
         <v>2250</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H21" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>57</v>
@@ -1597,17 +1597,29 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="1">
+        <v>45362</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.8520833333333333</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3">
+        <v>5000</v>
+      </c>
       <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+        <f>SUM(E23)-SUM(D23)</f>
+        <v>5000</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -4139,82 +4151,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3E639-FBD1-4498-B33D-4B47BAF93CDC}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="27" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>transaksi!M3</f>
-        <v>200000</v>
+        <v>55000</v>
       </c>
       <c r="B3" s="9">
         <v>91000</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="24">
+      <c r="A4" s="25">
         <f>B3+A3</f>
-        <v>291000</v>
-      </c>
-      <c r="B4" s="25"/>
+        <v>146000</v>
+      </c>
+      <c r="B4" s="26"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="E4" s="12">
+        <v>150000</v>
+      </c>
       <c r="F4" s="12">
         <v>65367</v>
       </c>
       <c r="G4" s="10">
         <f>SUM($A$4:$F$4)</f>
-        <v>356367</v>
+        <v>361367</v>
       </c>
       <c r="H4" s="11">
         <f>G4-$A$3</f>
-        <v>156367</v>
+        <v>306367</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -4257,8 +4271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509D0149-539F-4799-B8B7-7D5398715352}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4291,10 +4305,10 @@
       <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="32"/>
+      <c r="G1" s="33"/>
       <c r="H1" s="6" t="s">
         <v>14</v>
       </c>
@@ -4437,10 +4451,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="32"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -4454,9 +4468,9 @@
       <c r="F8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="16">
         <f>(transaksi!$K$3)*(H2/100)</f>
-        <v>30684.65625</v>
+        <v>34903.40625</v>
       </c>
       <c r="K8" t="s">
         <v>53</v>
@@ -4474,9 +4488,9 @@
       <c r="F9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="16">
         <f>(transaksi!$K$3)*(H3/100)</f>
-        <v>5682.34375</v>
+        <v>6463.59375</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
13 maret 24 - 10:12
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B8DF67-08A3-4B2F-B977-E8AE680CD046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9844E6-A553-44C9-9CF5-93A37D3A2213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transaksi" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
   <si>
     <t>Tanggal</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Juni</t>
+  </si>
+  <si>
+    <t>XL Xtra Htrd Spcl M, 7hr</t>
+  </si>
+  <si>
+    <t>tsel 10k</t>
   </si>
 </sst>
 </file>
@@ -559,10 +565,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -575,6 +587,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,22 +613,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,8 +942,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -994,31 +1001,31 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="17" t="s">
+      <c r="K1" s="30"/>
+      <c r="L1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="20" t="s">
+      <c r="M1" s="30"/>
+      <c r="N1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
       <c r="X1" t="s">
         <v>15</v>
       </c>
@@ -1065,17 +1072,17 @@
       <c r="M2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="S2" s="35" t="s">
+      <c r="N2" s="23"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="S2" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="T2" s="36">
+      <c r="T2" s="18">
         <v>1</v>
       </c>
-      <c r="U2" s="37">
+      <c r="U2" s="19">
         <f>SUM(F2:F5)</f>
         <v>7525</v>
       </c>
@@ -1111,23 +1118,23 @@
       </c>
       <c r="J3" s="5">
         <f>SUM($E$2:E201)</f>
-        <v>550000</v>
+        <v>577000</v>
       </c>
       <c r="K3" s="7">
         <f>SUM($F$2:F201)</f>
-        <v>48527</v>
+        <v>56317</v>
       </c>
       <c r="L3" s="5">
         <f>COUNTIF(H2:H201,TRUE)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M3" s="5">
         <f>SUMIF($H$2:$H$201,TRUE,$E$2:$E$201)</f>
-        <v>129000</v>
+        <v>144000</v>
       </c>
       <c r="N3" s="5">
         <f>wallet!G4</f>
-        <v>368527</v>
+        <v>376317</v>
       </c>
       <c r="O3" s="5">
         <f>deposit!G4</f>
@@ -1135,7 +1142,7 @@
       </c>
       <c r="P3" s="5">
         <f>SUM($D$2:$D$201)</f>
-        <v>501473</v>
+        <v>520683</v>
       </c>
       <c r="Q3" s="5" t="b">
         <f>((O3-P3)+J3) &lt;&gt; N3</f>
@@ -1144,11 +1151,11 @@
       <c r="R3" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="35"/>
-      <c r="T3" s="36">
+      <c r="S3" s="28"/>
+      <c r="T3" s="18">
         <v>2</v>
       </c>
-      <c r="U3" s="37"/>
+      <c r="U3" s="19"/>
       <c r="X3" t="s">
         <v>26</v>
       </c>
@@ -1182,11 +1189,11 @@
       <c r="I4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="35"/>
-      <c r="T4" s="36">
+      <c r="S4" s="28"/>
+      <c r="T4" s="18">
         <v>3</v>
       </c>
-      <c r="U4" s="37"/>
+      <c r="U4" s="19"/>
     </row>
     <row r="5" spans="1:29" ht="14.25" customHeight="1">
       <c r="A5" s="3">
@@ -1217,15 +1224,15 @@
       <c r="I5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="S5" s="35"/>
-      <c r="T5" s="36">
+      <c r="S5" s="28"/>
+      <c r="T5" s="18">
         <v>4</v>
       </c>
-      <c r="U5" s="37"/>
-      <c r="X5" s="32" t="s">
+      <c r="U5" s="19"/>
+      <c r="X5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Y5" s="19"/>
+      <c r="Y5" s="21"/>
       <c r="Z5" s="5"/>
     </row>
     <row r="6" spans="1:29" ht="14.25" customHeight="1">
@@ -1255,14 +1262,14 @@
         <v>0</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="S6" s="35" t="s">
+      <c r="S6" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="T6" s="36">
+      <c r="T6" s="18">
         <v>1</v>
       </c>
-      <c r="U6" s="37"/>
-      <c r="X6" s="33" t="s">
+      <c r="U6" s="19"/>
+      <c r="X6" s="17" t="s">
         <v>34</v>
       </c>
       <c r="Y6" s="5" t="s">
@@ -1297,12 +1304,12 @@
         <v>0</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="36">
+      <c r="S7" s="28"/>
+      <c r="T7" s="18">
         <v>2</v>
       </c>
-      <c r="U7" s="37"/>
-      <c r="X7" s="33" t="s">
+      <c r="U7" s="19"/>
+      <c r="X7" s="17" t="s">
         <v>36</v>
       </c>
       <c r="Y7" s="5" t="s">
@@ -1337,12 +1344,12 @@
         <v>0</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="36">
+      <c r="S8" s="28"/>
+      <c r="T8" s="18">
         <v>3</v>
       </c>
-      <c r="U8" s="37"/>
-      <c r="X8" s="33" t="s">
+      <c r="U8" s="19"/>
+      <c r="X8" s="17" t="s">
         <v>39</v>
       </c>
       <c r="Y8" s="5" t="s">
@@ -1376,11 +1383,11 @@
         <v>0</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="36">
+      <c r="S9" s="28"/>
+      <c r="T9" s="18">
         <v>4</v>
       </c>
-      <c r="U9" s="37"/>
+      <c r="U9" s="19"/>
     </row>
     <row r="10" spans="1:29" ht="14.25" customHeight="1">
       <c r="A10" s="3">
@@ -1409,13 +1416,13 @@
         <v>0</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="S10" s="35" t="s">
+      <c r="S10" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="T10" s="36">
+      <c r="T10" s="18">
         <v>1</v>
       </c>
-      <c r="U10" s="37"/>
+      <c r="U10" s="19"/>
     </row>
     <row r="11" spans="1:29" ht="14.25" customHeight="1">
       <c r="A11" s="3">
@@ -1444,11 +1451,11 @@
         <v>0</v>
       </c>
       <c r="I11" s="5"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="36">
+      <c r="S11" s="28"/>
+      <c r="T11" s="18">
         <v>2</v>
       </c>
-      <c r="U11" s="37"/>
+      <c r="U11" s="19"/>
     </row>
     <row r="12" spans="1:29" ht="14.25" customHeight="1">
       <c r="A12" s="3">
@@ -1477,11 +1484,11 @@
         <v>0</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="36">
+      <c r="S12" s="28"/>
+      <c r="T12" s="18">
         <v>3</v>
       </c>
-      <c r="U12" s="37"/>
+      <c r="U12" s="19"/>
     </row>
     <row r="13" spans="1:29" ht="14.25" customHeight="1">
       <c r="A13" s="3">
@@ -1508,11 +1515,11 @@
         <v>0</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="36">
+      <c r="S13" s="28"/>
+      <c r="T13" s="18">
         <v>4</v>
       </c>
-      <c r="U13" s="37"/>
+      <c r="U13" s="19"/>
     </row>
     <row r="14" spans="1:29" ht="14.25" customHeight="1">
       <c r="A14" s="3">
@@ -1541,13 +1548,13 @@
         <v>0</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="S14" s="35" t="s">
+      <c r="S14" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="T14" s="36">
+      <c r="T14" s="18">
         <v>1</v>
       </c>
-      <c r="U14" s="37"/>
+      <c r="U14" s="19"/>
     </row>
     <row r="15" spans="1:29" ht="14.25" customHeight="1">
       <c r="A15" s="3">
@@ -1578,11 +1585,11 @@
       <c r="I15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="S15" s="35"/>
-      <c r="T15" s="36">
+      <c r="S15" s="28"/>
+      <c r="T15" s="18">
         <v>2</v>
       </c>
-      <c r="U15" s="37"/>
+      <c r="U15" s="19"/>
     </row>
     <row r="16" spans="1:29" ht="14.25" customHeight="1">
       <c r="A16" s="3">
@@ -1613,11 +1620,11 @@
       <c r="I16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="35"/>
-      <c r="T16" s="36">
+      <c r="S16" s="28"/>
+      <c r="T16" s="18">
         <v>3</v>
       </c>
-      <c r="U16" s="37"/>
+      <c r="U16" s="19"/>
     </row>
     <row r="17" spans="1:21" ht="14.25" customHeight="1">
       <c r="A17" s="3">
@@ -1646,11 +1653,11 @@
         <v>0</v>
       </c>
       <c r="I17" s="5"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="36">
+      <c r="S17" s="28"/>
+      <c r="T17" s="18">
         <v>4</v>
       </c>
-      <c r="U17" s="37"/>
+      <c r="U17" s="19"/>
     </row>
     <row r="18" spans="1:21" ht="14.25" customHeight="1">
       <c r="A18" s="3">
@@ -1941,31 +1948,61 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="A28" s="3">
+        <v>45364</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="5">
+        <v>9000</v>
+      </c>
+      <c r="E28" s="5">
+        <v>15000</v>
+      </c>
       <c r="F28" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+        <v>6000</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="29" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="A29" s="3">
+        <v>45364</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="5">
+        <v>10210</v>
+      </c>
+      <c r="E29" s="5">
+        <v>12000</v>
+      </c>
       <c r="F29" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+        <v>1790</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:21" ht="14.25" customHeight="1">
@@ -4419,7 +4456,7 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4428,75 +4465,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
       <c r="A3" s="5">
         <f>transaksi!M3</f>
-        <v>129000</v>
+        <v>144000</v>
       </c>
       <c r="B3" s="8">
         <v>41000</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A4" s="27">
+      <c r="A4" s="33">
         <f>B3+A3</f>
-        <v>170000</v>
-      </c>
-      <c r="B4" s="18"/>
+        <v>185000</v>
+      </c>
+      <c r="B4" s="30"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="E4" s="9">
+        <v>12000</v>
+      </c>
       <c r="F4" s="9">
-        <v>198527</v>
+        <v>179317</v>
       </c>
       <c r="G4" s="10">
         <f>SUM($A$4:$F$4)</f>
-        <v>368527</v>
+        <v>376317</v>
       </c>
       <c r="H4" s="11">
         <f>G4-$A$3</f>
-        <v>239527</v>
+        <v>232317</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
@@ -4670,10 +4709,10 @@
       <c r="E1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="18"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="6" t="s">
         <v>64</v>
       </c>
@@ -4816,10 +4855,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -4835,7 +4874,7 @@
       </c>
       <c r="G8" s="15">
         <f>(transaksi!$K$3)*(H2/100)</f>
-        <v>40944.65625</v>
+        <v>47517.46875</v>
       </c>
       <c r="K8" t="s">
         <v>67</v>
@@ -4855,7 +4894,7 @@
       </c>
       <c r="G9" s="15">
         <f>(transaksi!$K$3)*(H3/100)</f>
-        <v>7582.34375</v>
+        <v>8799.53125</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
16 maret 24 - awal
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDB6AA4-2FC9-4BD7-A040-0F29C77F3E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92050F17-A9E0-4C8B-9916-2565DC637F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
   <si>
     <t>Tanggal</t>
   </si>
@@ -275,13 +275,22 @@
   </si>
   <si>
     <t>tsel 15k</t>
+  </si>
+  <si>
+    <t>indsat 10k</t>
+  </si>
+  <si>
+    <t>steam wallet 12k</t>
+  </si>
+  <si>
+    <t>saya pake koin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -311,6 +320,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -588,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -615,9 +636,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,11 +654,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -660,10 +681,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -680,7 +697,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,8 +938,8 @@
   <dimension ref="A1:AC401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -991,7 +1013,7 @@
       <c r="P1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="35" t="s">
         <v>14</v>
       </c>
       <c r="S1" s="36" t="s">
@@ -1045,11 +1067,11 @@
       <c r="M2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="35"/>
+      <c r="N2" s="34"/>
       <c r="O2" s="42"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="S2" s="45" t="s">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="S2" s="32" t="s">
         <v>24</v>
       </c>
       <c r="T2" s="8">
@@ -1091,23 +1113,23 @@
       </c>
       <c r="J3" s="6">
         <f>SUM($E$2:E201)</f>
-        <v>704000</v>
+        <v>722500</v>
       </c>
       <c r="K3" s="10">
         <f>SUM($F$2:F201)</f>
-        <v>57027</v>
+        <v>58270</v>
       </c>
       <c r="L3" s="6">
         <f>COUNTIF(H2:H201,TRUE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M3" s="6">
         <f>SUMIF($H$2:$H$201,TRUE,$E$2:$E$201)</f>
-        <v>57000</v>
+        <v>69000</v>
       </c>
       <c r="N3" s="6">
         <f>wallet!G4</f>
-        <v>377027</v>
+        <v>378270</v>
       </c>
       <c r="O3" s="6">
         <f>deposit!G4</f>
@@ -1115,7 +1137,7 @@
       </c>
       <c r="P3" s="6">
         <f>SUM($D$2:$D$201)</f>
-        <v>646973</v>
+        <v>664230</v>
       </c>
       <c r="Q3" s="6" t="b">
         <f>((O3-P3)+J3) &lt;&gt; N3</f>
@@ -1124,7 +1146,7 @@
       <c r="R3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="46"/>
+      <c r="S3" s="33"/>
       <c r="T3" s="8">
         <v>2</v>
       </c>
@@ -1157,12 +1179,12 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="46"/>
+      <c r="S4" s="33"/>
       <c r="T4" s="8">
         <v>3</v>
       </c>
@@ -1197,7 +1219,7 @@
       <c r="I5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="S5" s="35"/>
+      <c r="S5" s="34"/>
       <c r="T5" s="8">
         <v>4</v>
       </c>
@@ -1235,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="6"/>
-      <c r="S6" s="45" t="s">
+      <c r="S6" s="32" t="s">
         <v>36</v>
       </c>
       <c r="T6" s="8">
@@ -1277,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="6"/>
-      <c r="S7" s="46"/>
+      <c r="S7" s="33"/>
       <c r="T7" s="8">
         <v>2</v>
       </c>
@@ -1317,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="6"/>
-      <c r="S8" s="46"/>
+      <c r="S8" s="33"/>
       <c r="T8" s="8">
         <v>3</v>
       </c>
@@ -1356,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="6"/>
-      <c r="S9" s="35"/>
+      <c r="S9" s="34"/>
       <c r="T9" s="8">
         <v>4</v>
       </c>
@@ -1389,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="6"/>
-      <c r="S10" s="45" t="s">
+      <c r="S10" s="32" t="s">
         <v>44</v>
       </c>
       <c r="T10" s="8">
@@ -1424,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="6"/>
-      <c r="S11" s="46"/>
+      <c r="S11" s="33"/>
       <c r="T11" s="8">
         <v>2</v>
       </c>
@@ -1457,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="6"/>
-      <c r="S12" s="46"/>
+      <c r="S12" s="33"/>
       <c r="T12" s="8">
         <v>3</v>
       </c>
@@ -1490,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="S13" s="35"/>
+      <c r="S13" s="34"/>
       <c r="T13" s="8">
         <v>4</v>
       </c>
@@ -1525,7 +1547,7 @@
       <c r="I14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="S14" s="45" t="s">
+      <c r="S14" s="32" t="s">
         <v>48</v>
       </c>
       <c r="T14" s="8">
@@ -1562,7 +1584,7 @@
       <c r="I15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="S15" s="46"/>
+      <c r="S15" s="33"/>
       <c r="T15" s="8">
         <v>2</v>
       </c>
@@ -1595,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="6"/>
-      <c r="S16" s="46"/>
+      <c r="S16" s="33"/>
       <c r="T16" s="8">
         <v>3</v>
       </c>
@@ -1630,7 +1652,7 @@
       <c r="I17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="S17" s="35"/>
+      <c r="S17" s="34"/>
       <c r="T17" s="8">
         <v>4</v>
       </c>
@@ -1993,10 +2015,10 @@
       <c r="A30" s="18">
         <v>45366</v>
       </c>
-      <c r="B30" s="54">
-        <v>0.40486111111111112</v>
-      </c>
-      <c r="C30" s="33" t="s">
+      <c r="B30" s="52">
+        <v>0.34166666666666667</v>
+      </c>
+      <c r="C30" s="53" t="s">
         <v>83</v>
       </c>
       <c r="D30" s="19">
@@ -2018,32 +2040,62 @@
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="4">
+        <v>45367</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0.33611111111111114</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="6">
+        <v>10860</v>
+      </c>
+      <c r="E31" s="6">
+        <v>12000</v>
+      </c>
       <c r="F31" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
+        <v>1140</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="A32" s="4">
+        <v>45367</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="6">
+        <v>6397</v>
+      </c>
+      <c r="E32" s="6">
+        <v>6500</v>
+      </c>
       <c r="F32" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+        <v>103</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="14.25" customHeight="1">
       <c r="A33" s="4"/>
@@ -4657,7 +4709,7 @@
   <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4666,13 +4718,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="44"/>
       <c r="G1" s="40" t="s">
         <v>63</v>
@@ -4686,59 +4738,60 @@
         <v>65</v>
       </c>
       <c r="B2" s="38"/>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
       <c r="A3" s="6">
         <f>transaksi!M3</f>
-        <v>57000</v>
-      </c>
-      <c r="B3" s="20">
-        <v>84000</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+        <v>69000</v>
+      </c>
+      <c r="B3" s="55">
+        <f>90500</f>
+        <v>90500</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A4" s="47">
+      <c r="A4" s="45">
         <f>B3+A3</f>
-        <v>141000</v>
+        <v>159500</v>
       </c>
       <c r="B4" s="38"/>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>82000</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20">
         <v>101000</v>
       </c>
-      <c r="F4" s="21">
-        <v>53027</v>
-      </c>
-      <c r="G4" s="22">
+      <c r="F4" s="20">
+        <v>35770</v>
+      </c>
+      <c r="G4" s="21">
         <f>SUM($A$4:$F$4)</f>
-        <v>377027</v>
-      </c>
-      <c r="H4" s="23">
+        <v>378270</v>
+      </c>
+      <c r="H4" s="22">
         <f>G4-$A$3</f>
-        <v>320027</v>
+        <v>309270</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
@@ -4764,16 +4817,26 @@
     <row r="6" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:10" ht="14.25" customHeight="1">
+      <c r="J9">
+        <f>F4-14850</f>
+        <v>20920</v>
+      </c>
+    </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:10" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:10" ht="14.25" customHeight="1">
+      <c r="G16" s="56">
+        <f>42167-35770</f>
+        <v>6397</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -4980,15 +5043,15 @@
     <row r="220" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -5009,57 +5072,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
-      <c r="F3" s="27">
+      <c r="F3" s="26">
         <f t="shared" ref="F3:F4" si="0">SUM(B3:E3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
-      <c r="F4" s="27">
+      <c r="F4" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5067,12 +5130,12 @@
     <row r="5" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>75</v>
       </c>
     </row>
@@ -5181,9 +5244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L226"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5207,7 +5268,7 @@
       <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -5216,7 +5277,7 @@
       <c r="E1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>63</v>
       </c>
       <c r="G1" s="38"/>
@@ -5231,7 +5292,7 @@
       <c r="B2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="29">
         <v>51000</v>
       </c>
       <c r="D2" s="6">
@@ -5241,7 +5302,7 @@
         <f t="shared" ref="E2:E26" si="0">$C$2:$C$26-$D$2:$D$26</f>
         <v>50000</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>73</v>
       </c>
       <c r="G2" s="6">
@@ -5266,7 +5327,7 @@
       <c r="B3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="29">
         <v>51000</v>
       </c>
       <c r="D3" s="6">
@@ -5276,7 +5337,7 @@
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="30" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="6">
@@ -5301,7 +5362,7 @@
       <c r="B4" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>171000</v>
       </c>
       <c r="D4" s="6">
@@ -5311,7 +5372,7 @@
         <f t="shared" si="0"/>
         <v>170000</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="30" t="s">
         <v>63</v>
       </c>
       <c r="G4" s="6">
@@ -5332,7 +5393,7 @@
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <v>51000</v>
       </c>
       <c r="D5" s="6">
@@ -5346,7 +5407,7 @@
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="30"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6">
         <f t="shared" si="0"/>
@@ -5356,7 +5417,7 @@
     <row r="7" spans="1:12" ht="14.25" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="30"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
@@ -5370,7 +5431,7 @@
     <row r="8" spans="1:12" ht="14.25" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="30"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6">
         <f t="shared" si="0"/>
@@ -5379,9 +5440,9 @@
       <c r="F8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <f>(transaksi!$K$3)*(H2/100)</f>
-        <v>48116.53125</v>
+        <v>49165.3125</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>82</v>
@@ -5390,7 +5451,7 @@
     <row r="9" spans="1:12" ht="14.25" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="30"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6">
         <f t="shared" si="0"/>
@@ -5399,19 +5460,15 @@
       <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="31">
         <f>(transaksi!$K$3)*(H3/100)</f>
-        <v>8910.46875</v>
-      </c>
-      <c r="H9" s="55">
-        <f>G9-5000</f>
-        <v>3910.46875</v>
+        <v>9104.6875</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="30"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6">
         <f t="shared" si="0"/>
@@ -5421,7 +5478,7 @@
     <row r="11" spans="1:12" ht="14.25" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="30"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6">
         <f t="shared" si="0"/>
@@ -5431,7 +5488,7 @@
     <row r="12" spans="1:12" ht="14.25" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="30"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
         <f t="shared" si="0"/>
@@ -5441,7 +5498,7 @@
     <row r="13" spans="1:12" ht="14.25" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="30"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
         <f t="shared" si="0"/>
@@ -5451,7 +5508,7 @@
     <row r="14" spans="1:12" ht="14.25" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="30"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6">
         <f t="shared" si="0"/>
@@ -5461,7 +5518,7 @@
     <row r="15" spans="1:12" ht="14.25" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="30"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
         <f t="shared" si="0"/>
@@ -5471,7 +5528,7 @@
     <row r="16" spans="1:12" ht="14.25" customHeight="1">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="30"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6">
         <f t="shared" si="0"/>
@@ -5481,7 +5538,7 @@
     <row r="17" spans="1:5" ht="14.25" customHeight="1">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="30"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
@@ -5491,7 +5548,7 @@
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="30"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6">
         <f t="shared" si="0"/>
@@ -5501,7 +5558,7 @@
     <row r="19" spans="1:5" ht="14.25" customHeight="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="30"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
         <f t="shared" si="0"/>
@@ -5511,7 +5568,7 @@
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="30"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6">
         <f t="shared" si="0"/>
@@ -5521,7 +5578,7 @@
     <row r="21" spans="1:5" ht="14.25" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="30"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6">
         <f t="shared" si="0"/>
@@ -5531,7 +5588,7 @@
     <row r="22" spans="1:5" ht="14.25" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="30"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
         <f t="shared" si="0"/>
@@ -5541,7 +5598,7 @@
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="30"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6">
         <f t="shared" si="0"/>
@@ -5551,7 +5608,7 @@
     <row r="24" spans="1:5" ht="14.25" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="30"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6">
         <f t="shared" si="0"/>
@@ -5561,7 +5618,7 @@
     <row r="25" spans="1:5" ht="14.25" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="30"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6">
         <f t="shared" si="0"/>
@@ -5571,7 +5628,7 @@
     <row r="26" spans="1:5" ht="14.25" customHeight="1">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="30"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
akhir 17 maret 24
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6DD592-5BAC-43BF-9EA7-D31BCA288023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CDC1C6-A595-41BA-9EE4-C2DA00B62F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="93">
   <si>
     <t>Tanggal</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>Modal Terkumpul</t>
+  </si>
+  <si>
+    <t>tri 5k</t>
+  </si>
+  <si>
+    <t>axis 5k</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +386,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -658,14 +670,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -684,33 +689,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -719,6 +712,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,17 +747,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,7 +998,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
+      <selection pane="bottomLeft" activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1038,32 +1055,32 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="40" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="41"/>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="40" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="41"/>
-      <c r="N1" s="43" t="s">
+      <c r="N1" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="O1" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="40"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="61" t="s">
+      <c r="T1" s="38"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="30" t="s">
         <v>21</v>
       </c>
       <c r="X1" s="3" t="s">
@@ -1112,21 +1129,21 @@
       <c r="M2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="38"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="S2" s="48" t="s">
+      <c r="N2" s="35"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="S2" s="33" t="s">
         <v>23</v>
       </c>
       <c r="T2" s="8">
         <v>1</v>
       </c>
-      <c r="U2" s="58">
+      <c r="U2" s="27">
         <f>SUM(F2:F5)</f>
         <v>7525</v>
       </c>
-      <c r="V2" s="60">
+      <c r="V2" s="29">
         <f>COUNT($E$2:$E$5)</f>
         <v>4</v>
       </c>
@@ -1162,23 +1179,23 @@
       </c>
       <c r="J3" s="6">
         <f>SUM($E$2:E201)</f>
-        <v>755000</v>
+        <v>790000</v>
       </c>
       <c r="K3" s="9">
         <f>SUM($F$2:F201)</f>
-        <v>61770</v>
+        <v>68930</v>
       </c>
       <c r="L3" s="6">
         <f>COUNTIF(H2:H201,TRUE)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M3" s="6">
         <f>SUMIF($H$2:$H$201,TRUE,$E$2:$E$201)</f>
-        <v>96000</v>
+        <v>69000</v>
       </c>
       <c r="N3" s="6">
         <f>wallet!G4</f>
-        <v>381770</v>
+        <v>388930</v>
       </c>
       <c r="O3" s="6">
         <f>deposit!G4</f>
@@ -1186,7 +1203,7 @@
       </c>
       <c r="P3" s="6">
         <f>SUM($D$2:$D$201)</f>
-        <v>693230</v>
+        <v>721070</v>
       </c>
       <c r="Q3" s="6" t="b">
         <f>((O3-P3)+J3) &lt;&gt; N3</f>
@@ -1195,15 +1212,15 @@
       <c r="R3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="49"/>
+      <c r="S3" s="34"/>
       <c r="T3" s="8">
         <v>2</v>
       </c>
-      <c r="U3" s="58">
+      <c r="U3" s="27">
         <f>K3-U2</f>
-        <v>54245</v>
-      </c>
-      <c r="V3" s="60">
+        <v>61405</v>
+      </c>
+      <c r="V3" s="29">
         <f>COUNT($E$6:$E$35)</f>
         <v>30</v>
       </c>
@@ -1240,12 +1257,12 @@
       <c r="I4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="S4" s="49"/>
+      <c r="S4" s="34"/>
       <c r="T4" s="8">
         <v>3</v>
       </c>
-      <c r="U4" s="58"/>
-      <c r="V4" s="59"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="28"/>
     </row>
     <row r="5" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
@@ -1276,53 +1293,53 @@
       <c r="I5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="38"/>
+      <c r="S5" s="35"/>
       <c r="T5" s="8">
         <v>4</v>
       </c>
-      <c r="U5" s="58"/>
-      <c r="V5" s="59"/>
-      <c r="X5" s="46" t="s">
+      <c r="U5" s="27"/>
+      <c r="V5" s="28"/>
+      <c r="X5" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="Y5" s="47"/>
+      <c r="Y5" s="32"/>
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="52">
         <v>45361</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="53">
         <v>0.61250000000000004</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="54">
         <v>5850</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="54">
         <v>7000</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="54">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="S6" s="48" t="s">
+      <c r="H6" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="54"/>
+      <c r="S6" s="33" t="s">
         <v>35</v>
       </c>
       <c r="T6" s="8">
         <v>1</v>
       </c>
-      <c r="U6" s="58"/>
-      <c r="V6" s="59"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="28"/>
       <c r="X6" s="10" t="s">
         <v>36</v>
       </c>
@@ -1332,38 +1349,38 @@
       <c r="Z6" s="6"/>
     </row>
     <row r="7" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="52">
         <v>45361</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="53">
         <v>0.61458333333333337</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="54">
         <v>5850</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="54">
         <v>7000</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="54">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="S7" s="49"/>
+      <c r="H7" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="54"/>
+      <c r="S7" s="34"/>
       <c r="T7" s="8">
         <v>2</v>
       </c>
-      <c r="U7" s="58"/>
-      <c r="V7" s="59"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="28"/>
       <c r="X7" s="10" t="s">
         <v>38</v>
       </c>
@@ -1373,38 +1390,38 @@
       <c r="Z7" s="6"/>
     </row>
     <row r="8" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="52">
         <v>45361</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="53">
         <v>0.61527777777777781</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="54">
         <v>5275</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="54">
         <v>7000</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="54">
         <f t="shared" si="0"/>
         <v>1725</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="S8" s="49"/>
+      <c r="H8" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="54"/>
+      <c r="S8" s="34"/>
       <c r="T8" s="8">
         <v>3</v>
       </c>
-      <c r="U8" s="58"/>
-      <c r="V8" s="59"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="28"/>
       <c r="X8" s="10" t="s">
         <v>41</v>
       </c>
@@ -1413,408 +1430,408 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="52">
         <v>45361</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="53">
         <v>0.6166666666666667</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="54">
         <v>5850</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="54">
         <v>7000</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="54">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="S9" s="38"/>
+      <c r="H9" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="54"/>
+      <c r="S9" s="35"/>
       <c r="T9" s="8">
         <v>4</v>
       </c>
-      <c r="U9" s="58"/>
-      <c r="V9" s="59"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="28"/>
     </row>
     <row r="10" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="52">
         <v>45361</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="53">
         <v>0.6166666666666667</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="54">
         <v>5850</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="54">
         <v>7000</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="54">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="S10" s="48" t="s">
+      <c r="H10" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="54"/>
+      <c r="S10" s="33" t="s">
         <v>43</v>
       </c>
       <c r="T10" s="8">
         <v>1</v>
       </c>
-      <c r="U10" s="58"/>
-      <c r="V10" s="59"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="28"/>
     </row>
     <row r="11" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="52">
         <v>45361</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="53">
         <v>0.61736111111111114</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="54">
         <v>5275</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="54">
         <v>7000</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="54">
         <f t="shared" si="0"/>
         <v>1725</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="S11" s="49"/>
+      <c r="H11" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="54"/>
+      <c r="S11" s="34"/>
       <c r="T11" s="8">
         <v>2</v>
       </c>
-      <c r="U11" s="58"/>
-      <c r="V11" s="59"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="28"/>
     </row>
     <row r="12" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="52">
         <v>45361</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="53">
         <v>0.61736111111111114</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="54">
         <v>5850</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="54">
         <v>7000</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="54">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6"/>
-      <c r="S12" s="49"/>
+      <c r="H12" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="54"/>
+      <c r="S12" s="34"/>
       <c r="T12" s="8">
         <v>3</v>
       </c>
-      <c r="U12" s="58"/>
-      <c r="V12" s="59"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="28"/>
     </row>
     <row r="13" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+      <c r="A13" s="52">
         <v>45361</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="53">
         <v>0.77986111111111112</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="54">
         <v>10450</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="54">
         <v>12000</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="54">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="S13" s="38"/>
+      <c r="H13" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="54"/>
+      <c r="S13" s="35"/>
       <c r="T13" s="8">
         <v>4</v>
       </c>
-      <c r="U13" s="58"/>
-      <c r="V13" s="59"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="28"/>
     </row>
     <row r="14" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="A14" s="52">
         <v>45361</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="53">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="54">
         <v>58100</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="54">
         <v>62000</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="54">
         <f t="shared" si="0"/>
         <v>3900</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="48" t="s">
+      <c r="S14" s="33" t="s">
         <v>47</v>
       </c>
       <c r="T14" s="8">
         <v>1</v>
       </c>
-      <c r="U14" s="58"/>
-      <c r="V14" s="59"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="28"/>
     </row>
     <row r="15" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="A15" s="52">
         <v>45362</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="53">
         <v>0.37083333333333335</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="54">
         <v>29308</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="54">
         <v>31000</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="54">
         <f t="shared" si="0"/>
         <v>1692</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="S15" s="49"/>
+      <c r="S15" s="34"/>
       <c r="T15" s="8">
         <v>2</v>
       </c>
-      <c r="U15" s="58"/>
-      <c r="V15" s="59"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="28"/>
     </row>
     <row r="16" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="52">
         <v>45362</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="53">
         <v>0.38263888888888886</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="54">
         <v>50500</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="54">
         <v>52000</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="54">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6"/>
-      <c r="S16" s="49"/>
+      <c r="H16" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="54"/>
+      <c r="S16" s="34"/>
       <c r="T16" s="8">
         <v>3</v>
       </c>
-      <c r="U16" s="58"/>
-      <c r="V16" s="59"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="28"/>
     </row>
     <row r="17" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+      <c r="A17" s="52">
         <v>45362</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="53">
         <v>0.3923611111111111</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="54">
         <v>49750</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="54">
         <v>52000</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="54">
         <f t="shared" si="0"/>
         <v>2250</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="S17" s="38"/>
+      <c r="S17" s="35"/>
       <c r="T17" s="8">
         <v>4</v>
       </c>
-      <c r="U17" s="58"/>
-      <c r="V17" s="59"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="28"/>
     </row>
     <row r="18" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="A18" s="52">
         <v>45362</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="53">
         <v>0.39513888888888887</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="54">
         <v>12750</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="54">
         <v>14000</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="54">
         <f t="shared" si="0"/>
         <v>1250</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="6" t="b">
+      <c r="H18" s="54" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="54" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="A19" s="52">
         <v>45362</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="53">
         <v>0.40277777777777779</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="54">
         <v>49750</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="54">
         <v>52000</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="54">
         <f t="shared" si="0"/>
         <v>2250</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="54" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A20" s="52">
         <v>45362</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="53">
         <v>0.41458333333333336</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="54">
         <v>49750</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="54">
         <v>52000</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="54">
         <f t="shared" si="0"/>
         <v>2250</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="54" t="s">
         <v>46</v>
       </c>
       <c r="U20" t="s">
@@ -1822,508 +1839,578 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="52">
         <v>45362</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="53">
         <v>0.50486111111111109</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="54">
         <v>23000</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="54">
         <v>25000</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="54">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="6"/>
+      <c r="H21" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="A22" s="52">
         <v>45363</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="53">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="54">
         <v>10450</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="54">
         <v>12000</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="54">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="6"/>
+      <c r="H22" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="54"/>
     </row>
     <row r="23" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="52">
         <v>45364</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="53">
         <v>0.15069444444444444</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="54">
         <v>19890</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="54">
         <v>22000</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="54">
         <f t="shared" si="0"/>
         <v>2110</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="6" t="s">
+      <c r="H23" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="54" t="s">
         <v>56</v>
       </c>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="52">
         <v>45364</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="53">
         <v>0.25416666666666665</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="54">
         <v>50500</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="54">
         <v>52000</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="54">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="6" t="s">
+      <c r="H24" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="54" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="A25" s="52">
         <v>45364</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="53">
         <v>0.27083333333333331</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="54">
         <v>9000</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="54">
         <v>15000</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="54">
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="6" t="s">
+      <c r="H25" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="54" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
+      <c r="A26" s="55">
         <v>45364</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="56">
         <v>0.42222222222222222</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="57">
         <v>10210</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="57">
         <v>12000</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="54">
         <f t="shared" si="0"/>
         <v>1790</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="13"/>
+      <c r="H26" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="57"/>
     </row>
     <row r="27" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
+      <c r="A27" s="58">
         <v>45364</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="59">
         <v>0.91180555555555554</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="60">
         <v>12750</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="60">
         <v>14000</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="54">
         <f t="shared" si="0"/>
         <v>1250</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="16" t="b">
+      <c r="H27" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="I27" s="60" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
+      <c r="A28" s="58">
         <v>45364</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="59">
         <v>0.91597222222222219</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="60">
         <v>78800</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="60">
         <v>82000</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="54">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" s="16" t="s">
+      <c r="H28" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" s="60" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14">
+      <c r="A29" s="58">
         <v>45365</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="59">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="60">
         <v>19890</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="60">
         <v>22000</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="54">
         <f t="shared" si="0"/>
         <v>2110</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="G29" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="16"/>
+      <c r="H29" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="60"/>
     </row>
     <row r="30" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17">
+      <c r="A30" s="61">
         <v>45366</v>
       </c>
-      <c r="B30" s="31">
+      <c r="B30" s="62">
         <v>0.34166666666666667</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="64">
         <v>14850</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="64">
         <v>17000</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="54">
         <f t="shared" si="0"/>
         <v>2150</v>
       </c>
-      <c r="G30" s="18" t="s">
+      <c r="G30" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="18"/>
+      <c r="H30" s="64" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="64"/>
     </row>
     <row r="31" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+      <c r="A31" s="52">
         <v>45367</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="53">
         <v>0.33611111111111114</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="54">
         <v>10860</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="54">
         <v>12000</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="54">
         <f t="shared" si="0"/>
         <v>1140</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" s="6"/>
+      <c r="H31" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="54"/>
     </row>
     <row r="32" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+      <c r="A32" s="52">
         <v>45367</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="53">
         <v>0.35416666666666669</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="54">
         <v>6397</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="54">
         <v>6500</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="54">
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H32" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="33" t="s">
+      <c r="H32" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="65" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+      <c r="A33" s="52">
         <v>45367</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="53">
         <v>0.50486111111111109</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="54">
         <v>3300</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="54">
         <v>4000</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="54">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" s="6"/>
+      <c r="H33" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="54"/>
     </row>
     <row r="34" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
+      <c r="A34" s="52">
         <v>45367</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="53">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="54">
         <v>24600</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="54">
         <v>27000</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="54">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H34" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="6"/>
+      <c r="H34" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="54"/>
     </row>
     <row r="35" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+      <c r="A35" s="52">
         <v>45367</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="53">
         <v>0.55694444444444446</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="54">
         <v>1100</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="54">
         <v>1500</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="54">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G35" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" s="33" t="s">
+      <c r="H35" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="65" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="A36" s="4">
+        <v>45368</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0.96944444444444444</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="6">
+        <v>5275</v>
+      </c>
+      <c r="E36" s="6">
+        <v>7000</v>
+      </c>
       <c r="F36" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
+        <v>1725</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="A37" s="4">
+        <v>45368</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0.96944444444444444</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="6">
+        <v>5570</v>
+      </c>
+      <c r="E37" s="6">
+        <v>7000</v>
+      </c>
       <c r="F37" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
+        <v>1430</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I37" s="6"/>
     </row>
     <row r="38" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="A38" s="4">
+        <v>45368</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0.96944444444444444</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="6">
+        <v>5870</v>
+      </c>
+      <c r="E38" s="6">
+        <v>7000</v>
+      </c>
       <c r="F38" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
+        <v>1130</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I38" s="6"/>
     </row>
     <row r="39" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="A39" s="4">
+        <v>45368</v>
+      </c>
+      <c r="B39" s="5">
+        <v>0.96944444444444444</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="6">
+        <v>5850</v>
+      </c>
+      <c r="E39" s="6">
+        <v>7000</v>
+      </c>
       <c r="F39" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
+        <v>1150</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="A40" s="4">
+        <v>45368</v>
+      </c>
+      <c r="B40" s="5">
+        <v>0.96944444444444444</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="6">
+        <v>5275</v>
+      </c>
+      <c r="E40" s="6">
+        <v>7000</v>
+      </c>
       <c r="F40" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
+        <v>1725</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H40" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4782,11 +4869,6 @@
     <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="S6:S9"/>
-    <mergeCell ref="S2:S5"/>
-    <mergeCell ref="S10:S13"/>
-    <mergeCell ref="S14:S17"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="J1:K1"/>
@@ -4794,6 +4876,11 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="S6:S9"/>
+    <mergeCell ref="S2:S5"/>
+    <mergeCell ref="S10:S13"/>
+    <mergeCell ref="S14:S17"/>
   </mergeCells>
   <conditionalFormatting sqref="M3">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -4826,7 +4913,7 @@
   <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4835,80 +4922,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="43" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="42" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="41"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f>transaksi!M3</f>
-        <v>96000</v>
-      </c>
-      <c r="B3" s="34">
+        <v>69000</v>
+      </c>
+      <c r="B3" s="24">
         <f>86000</f>
         <v>86000</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50">
+      <c r="A4" s="45">
         <f>B3+A3</f>
-        <v>182000</v>
+        <v>155000</v>
       </c>
       <c r="B4" s="41"/>
-      <c r="C4" s="19">
-        <v>0</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19">
-        <v>50000</v>
-      </c>
-      <c r="F4" s="19">
-        <v>149770</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12">
+        <v>112000</v>
+      </c>
+      <c r="F4" s="12">
+        <v>121930</v>
+      </c>
+      <c r="G4" s="13">
         <f>SUM($A$4:$F$4)</f>
-        <v>381770</v>
-      </c>
-      <c r="H4" s="21">
+        <v>388930</v>
+      </c>
+      <c r="H4" s="14">
         <f>G4-$A$3</f>
-        <v>285770</v>
+        <v>319930</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4934,7 +5021,7 @@
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="22"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4944,7 +5031,7 @@
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="35"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5181,57 +5268,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="17" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="18">
         <f t="shared" ref="F3:F4" si="0">SUM(B3:E3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="25">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5239,12 +5326,12 @@
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="19" t="s">
         <v>74</v>
       </c>
     </row>
@@ -5377,7 +5464,7 @@
       <c r="B1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -5386,7 +5473,7 @@
       <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="51" t="s">
         <v>62</v>
       </c>
       <c r="G1" s="41"/>
@@ -5401,7 +5488,7 @@
       <c r="B2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="21">
         <v>51000</v>
       </c>
       <c r="D2" s="6">
@@ -5411,7 +5498,7 @@
         <f t="shared" ref="E2:E26" si="0">$C$2:$C$26-$D$2:$D$26</f>
         <v>50000</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="22" t="s">
         <v>72</v>
       </c>
       <c r="G2" s="6">
@@ -5436,7 +5523,7 @@
       <c r="B3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="21">
         <v>51000</v>
       </c>
       <c r="D3" s="6">
@@ -5446,7 +5533,7 @@
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="22" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="6">
@@ -5471,7 +5558,7 @@
       <c r="B4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="21">
         <v>171000</v>
       </c>
       <c r="D4" s="6">
@@ -5481,7 +5568,7 @@
         <f t="shared" si="0"/>
         <v>170000</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="22" t="s">
         <v>62</v>
       </c>
       <c r="G4" s="6">
@@ -5502,7 +5589,7 @@
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="21">
         <v>51000</v>
       </c>
       <c r="D5" s="6">
@@ -5516,7 +5603,7 @@
     <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="28"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6">
         <f t="shared" si="0"/>
@@ -5526,13 +5613,13 @@
     <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="28"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="40" t="s">
         <v>80</v>
       </c>
       <c r="G7" s="41"/>
@@ -5540,7 +5627,7 @@
     <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="28"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6">
         <f t="shared" si="0"/>
@@ -5549,9 +5636,9 @@
       <c r="F8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="23">
         <f>(transaksi!$K$3)*(H2/100)</f>
-        <v>52118.4375</v>
+        <v>58159.6875</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>81</v>
@@ -5560,7 +5647,7 @@
     <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="28"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6">
         <f t="shared" si="0"/>
@@ -5569,15 +5656,15 @@
       <c r="F9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="23">
         <f>(transaksi!$K$3)*(H3/100)</f>
-        <v>9651.5625</v>
+        <v>10770.3125</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="28"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6">
         <f t="shared" si="0"/>
@@ -5587,7 +5674,7 @@
     <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="28"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6">
         <f t="shared" si="0"/>
@@ -5597,7 +5684,7 @@
     <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="28"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6">
         <f t="shared" si="0"/>
@@ -5607,7 +5694,7 @@
     <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="28"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
         <f t="shared" si="0"/>
@@ -5617,7 +5704,7 @@
     <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="28"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6">
         <f t="shared" si="0"/>
@@ -5627,7 +5714,7 @@
     <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="28"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
         <f t="shared" si="0"/>
@@ -5637,7 +5724,7 @@
     <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="28"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6">
         <f t="shared" si="0"/>
@@ -5647,7 +5734,7 @@
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="28"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
@@ -5657,7 +5744,7 @@
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="28"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6">
         <f t="shared" si="0"/>
@@ -5667,7 +5754,7 @@
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="28"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
         <f t="shared" si="0"/>
@@ -5677,7 +5764,7 @@
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="28"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6">
         <f t="shared" si="0"/>
@@ -5687,7 +5774,7 @@
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="28"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6">
         <f t="shared" si="0"/>
@@ -5697,7 +5784,7 @@
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="28"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
         <f t="shared" si="0"/>
@@ -5707,7 +5794,7 @@
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="28"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6">
         <f t="shared" si="0"/>
@@ -5717,7 +5804,7 @@
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="28"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6">
         <f t="shared" si="0"/>
@@ -5727,7 +5814,7 @@
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="28"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6">
         <f t="shared" si="0"/>
@@ -5737,7 +5824,7 @@
     <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="28"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
mulai 19 maret 24 (+1)
</commit_message>
<xml_diff>
--- a/transaksi-usaha.xlsx
+++ b/transaksi-usaha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Tugas\Kewirausahaan\transaksi-usaha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CDC1C6-A595-41BA-9EE4-C2DA00B62F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18B25CE-9F75-4292-8C00-21FBFEE42832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
   <si>
     <t>Tanggal</t>
   </si>
@@ -302,6 +302,12 @@
   </si>
   <si>
     <t>axis 5k</t>
+  </si>
+  <si>
+    <t>indsat 5GB/5hr</t>
+  </si>
+  <si>
+    <t>aby</t>
   </si>
 </sst>
 </file>
@@ -654,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -704,18 +710,25 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -732,6 +745,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -747,21 +768,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,8 +1004,8 @@
   <dimension ref="A1:AC401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q43" sqref="Q43"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1055,35 +1062,35 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="41"/>
-      <c r="L1" s="40" t="s">
+      <c r="K1" s="52"/>
+      <c r="L1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="41"/>
-      <c r="N1" s="42" t="s">
+      <c r="M1" s="52"/>
+      <c r="N1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="43" t="s">
+      <c r="O1" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="38"/>
-      <c r="U1" s="39"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="50"/>
       <c r="V1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="67" t="s">
         <v>15</v>
       </c>
       <c r="AC1" s="3" t="s">
@@ -1129,11 +1136,11 @@
       <c r="M2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="S2" s="33" t="s">
+      <c r="N2" s="47"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="S2" s="58" t="s">
         <v>23</v>
       </c>
       <c r="T2" s="8">
@@ -1179,23 +1186,23 @@
       </c>
       <c r="J3" s="6">
         <f>SUM($E$2:E201)</f>
-        <v>790000</v>
+        <v>832000</v>
       </c>
       <c r="K3" s="9">
         <f>SUM($F$2:F201)</f>
-        <v>68930</v>
+        <v>72290</v>
       </c>
       <c r="L3" s="6">
         <f>COUNTIF(H2:H201,TRUE)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M3" s="6">
         <f>SUMIF($H$2:$H$201,TRUE,$E$2:$E$201)</f>
-        <v>69000</v>
+        <v>89000</v>
       </c>
       <c r="N3" s="6">
         <f>wallet!G4</f>
-        <v>388930</v>
+        <v>392290</v>
       </c>
       <c r="O3" s="6">
         <f>deposit!G4</f>
@@ -1203,7 +1210,7 @@
       </c>
       <c r="P3" s="6">
         <f>SUM($D$2:$D$201)</f>
-        <v>721070</v>
+        <v>759710</v>
       </c>
       <c r="Q3" s="6" t="b">
         <f>((O3-P3)+J3) &lt;&gt; N3</f>
@@ -1212,13 +1219,13 @@
       <c r="R3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="34"/>
+      <c r="S3" s="59"/>
       <c r="T3" s="8">
         <v>2</v>
       </c>
       <c r="U3" s="27">
         <f>K3-U2</f>
-        <v>61405</v>
+        <v>64765</v>
       </c>
       <c r="V3" s="29">
         <f>COUNT($E$6:$E$35)</f>
@@ -1257,7 +1264,7 @@
       <c r="I4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="S4" s="34"/>
+      <c r="S4" s="59"/>
       <c r="T4" s="8">
         <v>3</v>
       </c>
@@ -1293,46 +1300,46 @@
       <c r="I5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="35"/>
+      <c r="S5" s="47"/>
       <c r="T5" s="8">
         <v>4</v>
       </c>
       <c r="U5" s="27"/>
       <c r="V5" s="28"/>
-      <c r="X5" s="31" t="s">
+      <c r="X5" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="Y5" s="32"/>
+      <c r="Y5" s="57"/>
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="52">
+      <c r="A6" s="31">
         <v>45361</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="32">
         <v>0.61250000000000004</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="33">
         <v>5850</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="33">
         <v>7000</v>
       </c>
-      <c r="F6" s="54">
+      <c r="F6" s="33">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="54"/>
-      <c r="S6" s="33" t="s">
+      <c r="H6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="33"/>
+      <c r="S6" s="58" t="s">
         <v>35</v>
       </c>
       <c r="T6" s="8">
@@ -1349,33 +1356,33 @@
       <c r="Z6" s="6"/>
     </row>
     <row r="7" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52">
+      <c r="A7" s="31">
         <v>45361</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="32">
         <v>0.61458333333333337</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="33">
         <v>5850</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="33">
         <v>7000</v>
       </c>
-      <c r="F7" s="54">
+      <c r="F7" s="33">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="54"/>
-      <c r="S7" s="34"/>
+      <c r="H7" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="33"/>
+      <c r="S7" s="59"/>
       <c r="T7" s="8">
         <v>2</v>
       </c>
@@ -1390,33 +1397,33 @@
       <c r="Z7" s="6"/>
     </row>
     <row r="8" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52">
+      <c r="A8" s="31">
         <v>45361</v>
       </c>
-      <c r="B8" s="53">
+      <c r="B8" s="32">
         <v>0.61527777777777781</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="54">
+      <c r="D8" s="33">
         <v>5275</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="33">
         <v>7000</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="33">
         <f t="shared" si="0"/>
         <v>1725</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="54"/>
-      <c r="S8" s="34"/>
+      <c r="H8" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="33"/>
+      <c r="S8" s="59"/>
       <c r="T8" s="8">
         <v>3</v>
       </c>
@@ -1430,33 +1437,33 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="52">
+      <c r="A9" s="31">
         <v>45361</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="32">
         <v>0.6166666666666667</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="54">
+      <c r="D9" s="33">
         <v>5850</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="33">
         <v>7000</v>
       </c>
-      <c r="F9" s="54">
+      <c r="F9" s="33">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G9" s="54" t="s">
+      <c r="G9" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="54"/>
-      <c r="S9" s="35"/>
+      <c r="H9" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="33"/>
+      <c r="S9" s="47"/>
       <c r="T9" s="8">
         <v>4</v>
       </c>
@@ -1464,33 +1471,33 @@
       <c r="V9" s="28"/>
     </row>
     <row r="10" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52">
+      <c r="A10" s="31">
         <v>45361</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="32">
         <v>0.6166666666666667</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="33">
         <v>5850</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="33">
         <v>7000</v>
       </c>
-      <c r="F10" s="54">
+      <c r="F10" s="33">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="54"/>
-      <c r="S10" s="33" t="s">
+      <c r="H10" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="33"/>
+      <c r="S10" s="58" t="s">
         <v>43</v>
       </c>
       <c r="T10" s="8">
@@ -1500,33 +1507,33 @@
       <c r="V10" s="28"/>
     </row>
     <row r="11" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="52">
+      <c r="A11" s="31">
         <v>45361</v>
       </c>
-      <c r="B11" s="53">
+      <c r="B11" s="32">
         <v>0.61736111111111114</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="33">
         <v>5275</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="33">
         <v>7000</v>
       </c>
-      <c r="F11" s="54">
+      <c r="F11" s="33">
         <f t="shared" si="0"/>
         <v>1725</v>
       </c>
-      <c r="G11" s="54" t="s">
+      <c r="G11" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="54"/>
-      <c r="S11" s="34"/>
+      <c r="H11" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33"/>
+      <c r="S11" s="59"/>
       <c r="T11" s="8">
         <v>2</v>
       </c>
@@ -1534,33 +1541,33 @@
       <c r="V11" s="28"/>
     </row>
     <row r="12" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52">
+      <c r="A12" s="31">
         <v>45361</v>
       </c>
-      <c r="B12" s="53">
+      <c r="B12" s="32">
         <v>0.61736111111111114</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="33">
         <v>5850</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="33">
         <v>7000</v>
       </c>
-      <c r="F12" s="54">
+      <c r="F12" s="33">
         <f t="shared" si="0"/>
         <v>1150</v>
       </c>
-      <c r="G12" s="54" t="s">
+      <c r="G12" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="54"/>
-      <c r="S12" s="34"/>
+      <c r="H12" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="33"/>
+      <c r="S12" s="59"/>
       <c r="T12" s="8">
         <v>3</v>
       </c>
@@ -1568,33 +1575,33 @@
       <c r="V12" s="28"/>
     </row>
     <row r="13" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52">
+      <c r="A13" s="31">
         <v>45361</v>
       </c>
-      <c r="B13" s="53">
+      <c r="B13" s="32">
         <v>0.77986111111111112</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="33">
         <v>10450</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="33">
         <v>12000</v>
       </c>
-      <c r="F13" s="54">
+      <c r="F13" s="33">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
-      <c r="G13" s="54" t="s">
+      <c r="G13" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="54"/>
-      <c r="S13" s="35"/>
+      <c r="H13" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33"/>
+      <c r="S13" s="47"/>
       <c r="T13" s="8">
         <v>4</v>
       </c>
@@ -1602,35 +1609,35 @@
       <c r="V13" s="28"/>
     </row>
     <row r="14" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52">
+      <c r="A14" s="31">
         <v>45361</v>
       </c>
-      <c r="B14" s="53">
+      <c r="B14" s="32">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="33">
         <v>58100</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="33">
         <v>62000</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="33">
         <f t="shared" si="0"/>
         <v>3900</v>
       </c>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="54" t="s">
+      <c r="H14" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="33" t="s">
+      <c r="S14" s="58" t="s">
         <v>47</v>
       </c>
       <c r="T14" s="8">
@@ -1640,35 +1647,35 @@
       <c r="V14" s="28"/>
     </row>
     <row r="15" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52">
+      <c r="A15" s="31">
         <v>45362</v>
       </c>
-      <c r="B15" s="53">
+      <c r="B15" s="32">
         <v>0.37083333333333335</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="33">
         <v>29308</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="33">
         <v>31000</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="33">
         <f t="shared" si="0"/>
         <v>1692</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="54" t="s">
+      <c r="H15" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="S15" s="34"/>
+      <c r="S15" s="59"/>
       <c r="T15" s="8">
         <v>2</v>
       </c>
@@ -1676,33 +1683,33 @@
       <c r="V15" s="28"/>
     </row>
     <row r="16" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="52">
+      <c r="A16" s="31">
         <v>45362</v>
       </c>
-      <c r="B16" s="53">
+      <c r="B16" s="32">
         <v>0.38263888888888886</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="54">
+      <c r="D16" s="33">
         <v>50500</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="33">
         <v>52000</v>
       </c>
-      <c r="F16" s="54">
+      <c r="F16" s="33">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="G16" s="54" t="s">
+      <c r="G16" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="54"/>
-      <c r="S16" s="34"/>
+      <c r="H16" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="33"/>
+      <c r="S16" s="59"/>
       <c r="T16" s="8">
         <v>3</v>
       </c>
@@ -1710,35 +1717,35 @@
       <c r="V16" s="28"/>
     </row>
     <row r="17" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52">
+      <c r="A17" s="31">
         <v>45362</v>
       </c>
-      <c r="B17" s="53">
+      <c r="B17" s="32">
         <v>0.3923611111111111</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D17" s="33">
         <v>49750</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="33">
         <v>52000</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="33">
         <f t="shared" si="0"/>
         <v>2250</v>
       </c>
-      <c r="G17" s="54" t="s">
+      <c r="G17" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="54" t="s">
+      <c r="H17" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="S17" s="35"/>
+      <c r="S17" s="47"/>
       <c r="T17" s="8">
         <v>4</v>
       </c>
@@ -1746,92 +1753,92 @@
       <c r="V17" s="28"/>
     </row>
     <row r="18" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52">
+      <c r="A18" s="31">
         <v>45362</v>
       </c>
-      <c r="B18" s="53">
+      <c r="B18" s="32">
         <v>0.39513888888888887</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="54">
+      <c r="D18" s="33">
         <v>12750</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="33">
         <v>14000</v>
       </c>
-      <c r="F18" s="54">
+      <c r="F18" s="33">
         <f t="shared" si="0"/>
         <v>1250</v>
       </c>
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="54" t="b">
+      <c r="H18" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="54" t="s">
+      <c r="I18" s="33" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="52">
+      <c r="A19" s="31">
         <v>45362</v>
       </c>
-      <c r="B19" s="53">
+      <c r="B19" s="32">
         <v>0.40277777777777779</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="33">
         <v>49750</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="33">
         <v>52000</v>
       </c>
-      <c r="F19" s="54">
+      <c r="F19" s="33">
         <f t="shared" si="0"/>
         <v>2250</v>
       </c>
-      <c r="G19" s="54" t="s">
+      <c r="G19" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="54" t="s">
+      <c r="H19" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="33" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="52">
+      <c r="A20" s="31">
         <v>45362</v>
       </c>
-      <c r="B20" s="53">
+      <c r="B20" s="32">
         <v>0.41458333333333336</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="54">
+      <c r="D20" s="33">
         <v>49750</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="33">
         <v>52000</v>
       </c>
-      <c r="F20" s="54">
+      <c r="F20" s="33">
         <f t="shared" si="0"/>
         <v>2250</v>
       </c>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="54" t="s">
+      <c r="H20" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="33" t="s">
         <v>46</v>
       </c>
       <c r="U20" t="s">
@@ -1839,437 +1846,437 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52">
+      <c r="A21" s="31">
         <v>45362</v>
       </c>
-      <c r="B21" s="53">
+      <c r="B21" s="32">
         <v>0.50486111111111109</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="54">
+      <c r="D21" s="33">
         <v>23000</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="33">
         <v>25000</v>
       </c>
-      <c r="F21" s="54">
+      <c r="F21" s="33">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="G21" s="54" t="s">
+      <c r="G21" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="54"/>
+      <c r="H21" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="33"/>
     </row>
     <row r="22" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52">
+      <c r="A22" s="31">
         <v>45363</v>
       </c>
-      <c r="B22" s="53">
+      <c r="B22" s="32">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="54">
+      <c r="D22" s="33">
         <v>10450</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="33">
         <v>12000</v>
       </c>
-      <c r="F22" s="54">
+      <c r="F22" s="33">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
-      <c r="G22" s="54" t="s">
+      <c r="G22" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="54"/>
+      <c r="H22" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="33"/>
     </row>
     <row r="23" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52">
+      <c r="A23" s="31">
         <v>45364</v>
       </c>
-      <c r="B23" s="53">
+      <c r="B23" s="32">
         <v>0.15069444444444444</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="54">
+      <c r="D23" s="33">
         <v>19890</v>
       </c>
-      <c r="E23" s="54">
+      <c r="E23" s="33">
         <v>22000</v>
       </c>
-      <c r="F23" s="54">
+      <c r="F23" s="33">
         <f t="shared" si="0"/>
         <v>2110</v>
       </c>
-      <c r="G23" s="54" t="s">
+      <c r="G23" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="54" t="s">
+      <c r="H23" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="33" t="s">
         <v>56</v>
       </c>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="52">
+      <c r="A24" s="31">
         <v>45364</v>
       </c>
-      <c r="B24" s="53">
+      <c r="B24" s="32">
         <v>0.25416666666666665</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="54">
+      <c r="D24" s="33">
         <v>50500</v>
       </c>
-      <c r="E24" s="54">
+      <c r="E24" s="33">
         <v>52000</v>
       </c>
-      <c r="F24" s="54">
+      <c r="F24" s="33">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="G24" s="54" t="s">
+      <c r="G24" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="54" t="s">
+      <c r="H24" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="52">
+      <c r="A25" s="31">
         <v>45364</v>
       </c>
-      <c r="B25" s="53">
+      <c r="B25" s="32">
         <v>0.27083333333333331</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="54">
+      <c r="D25" s="33">
         <v>9000</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="33">
         <v>15000</v>
       </c>
-      <c r="F25" s="54">
+      <c r="F25" s="33">
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
-      <c r="G25" s="54" t="s">
+      <c r="G25" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="54" t="s">
+      <c r="H25" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="55">
+      <c r="A26" s="34">
         <v>45364</v>
       </c>
-      <c r="B26" s="56">
+      <c r="B26" s="35">
         <v>0.42222222222222222</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="57">
+      <c r="D26" s="36">
         <v>10210</v>
       </c>
-      <c r="E26" s="57">
+      <c r="E26" s="36">
         <v>12000</v>
       </c>
-      <c r="F26" s="54">
+      <c r="F26" s="33">
         <f t="shared" si="0"/>
         <v>1790</v>
       </c>
-      <c r="G26" s="57" t="s">
+      <c r="G26" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="57" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="57"/>
+      <c r="H26" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="36"/>
     </row>
     <row r="27" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="58">
+      <c r="A27" s="37">
         <v>45364</v>
       </c>
-      <c r="B27" s="59">
+      <c r="B27" s="38">
         <v>0.91180555555555554</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="60">
+      <c r="D27" s="39">
         <v>12750</v>
       </c>
-      <c r="E27" s="60">
+      <c r="E27" s="39">
         <v>14000</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F27" s="33">
         <f t="shared" si="0"/>
         <v>1250</v>
       </c>
-      <c r="G27" s="60" t="s">
+      <c r="G27" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="60" t="b">
+      <c r="H27" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="I27" s="60" t="s">
+      <c r="I27" s="39" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="58">
+      <c r="A28" s="37">
         <v>45364</v>
       </c>
-      <c r="B28" s="59">
+      <c r="B28" s="38">
         <v>0.91597222222222219</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="60">
+      <c r="D28" s="39">
         <v>78800</v>
       </c>
-      <c r="E28" s="60">
+      <c r="E28" s="39">
         <v>82000</v>
       </c>
-      <c r="F28" s="54">
+      <c r="F28" s="33">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
-      <c r="G28" s="60" t="s">
+      <c r="G28" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" s="60" t="s">
+      <c r="H28" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" s="39" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="58">
+      <c r="A29" s="37">
         <v>45365</v>
       </c>
-      <c r="B29" s="59">
+      <c r="B29" s="38">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="60">
+      <c r="D29" s="39">
         <v>19890</v>
       </c>
-      <c r="E29" s="60">
+      <c r="E29" s="39">
         <v>22000</v>
       </c>
-      <c r="F29" s="54">
+      <c r="F29" s="33">
         <f t="shared" si="0"/>
         <v>2110</v>
       </c>
-      <c r="G29" s="60" t="s">
+      <c r="G29" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="60"/>
+      <c r="H29" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="39"/>
     </row>
     <row r="30" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="61">
+      <c r="A30" s="40">
         <v>45366</v>
       </c>
-      <c r="B30" s="62">
+      <c r="B30" s="41">
         <v>0.34166666666666667</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="64">
+      <c r="D30" s="43">
         <v>14850</v>
       </c>
-      <c r="E30" s="64">
+      <c r="E30" s="43">
         <v>17000</v>
       </c>
-      <c r="F30" s="54">
+      <c r="F30" s="33">
         <f t="shared" si="0"/>
         <v>2150</v>
       </c>
-      <c r="G30" s="64" t="s">
+      <c r="G30" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="64" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="64"/>
+      <c r="H30" s="43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="43"/>
     </row>
     <row r="31" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="52">
+      <c r="A31" s="31">
         <v>45367</v>
       </c>
-      <c r="B31" s="53">
+      <c r="B31" s="32">
         <v>0.33611111111111114</v>
       </c>
-      <c r="C31" s="65" t="s">
+      <c r="C31" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="54">
+      <c r="D31" s="33">
         <v>10860</v>
       </c>
-      <c r="E31" s="54">
+      <c r="E31" s="33">
         <v>12000</v>
       </c>
-      <c r="F31" s="54">
+      <c r="F31" s="33">
         <f t="shared" si="0"/>
         <v>1140</v>
       </c>
-      <c r="G31" s="54" t="s">
+      <c r="G31" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" s="54"/>
+      <c r="H31" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="33"/>
     </row>
     <row r="32" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="52">
+      <c r="A32" s="31">
         <v>45367</v>
       </c>
-      <c r="B32" s="53">
+      <c r="B32" s="32">
         <v>0.35416666666666669</v>
       </c>
-      <c r="C32" s="65" t="s">
+      <c r="C32" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="54">
+      <c r="D32" s="33">
         <v>6397</v>
       </c>
-      <c r="E32" s="54">
+      <c r="E32" s="33">
         <v>6500</v>
       </c>
-      <c r="F32" s="54">
+      <c r="F32" s="33">
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="G32" s="54" t="s">
+      <c r="G32" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H32" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="65" t="s">
+      <c r="H32" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="44" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="52">
+      <c r="A33" s="31">
         <v>45367</v>
       </c>
-      <c r="B33" s="53">
+      <c r="B33" s="32">
         <v>0.50486111111111109</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="54">
+      <c r="D33" s="33">
         <v>3300</v>
       </c>
-      <c r="E33" s="54">
+      <c r="E33" s="33">
         <v>4000</v>
       </c>
-      <c r="F33" s="54">
+      <c r="F33" s="33">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="G33" s="54" t="s">
+      <c r="G33" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" s="54"/>
+      <c r="H33" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="33"/>
     </row>
     <row r="34" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="52">
+      <c r="A34" s="31">
         <v>45367</v>
       </c>
-      <c r="B34" s="53">
+      <c r="B34" s="32">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C34" s="65" t="s">
+      <c r="C34" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="54">
+      <c r="D34" s="33">
         <v>24600</v>
       </c>
-      <c r="E34" s="54">
+      <c r="E34" s="33">
         <v>27000</v>
       </c>
-      <c r="F34" s="54">
+      <c r="F34" s="33">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="G34" s="54" t="s">
+      <c r="G34" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H34" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" s="54"/>
+      <c r="H34" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33"/>
     </row>
     <row r="35" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="52">
+      <c r="A35" s="31">
         <v>45367</v>
       </c>
-      <c r="B35" s="53">
+      <c r="B35" s="32">
         <v>0.55694444444444446</v>
       </c>
-      <c r="C35" s="65" t="s">
+      <c r="C35" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="54">
+      <c r="D35" s="33">
         <v>1100</v>
       </c>
-      <c r="E35" s="54">
+      <c r="E35" s="33">
         <v>1500</v>
       </c>
-      <c r="F35" s="54">
+      <c r="F35" s="33">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="G35" s="54" t="s">
+      <c r="G35" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" s="65" t="s">
+      <c r="H35" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="44" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2414,31 +2421,61 @@
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="A41" s="4">
+        <v>45370</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0.3125</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="6">
+        <v>18750</v>
+      </c>
+      <c r="E41" s="6">
+        <v>20000</v>
+      </c>
       <c r="F41" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
+        <v>1250</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="42" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="A42" s="4">
+        <v>45369</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="6">
+        <v>19890</v>
+      </c>
+      <c r="E42" s="6">
+        <v>22000</v>
+      </c>
       <c r="F42" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
+        <v>2110</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4869,6 +4906,11 @@
     <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="S6:S9"/>
+    <mergeCell ref="S2:S5"/>
+    <mergeCell ref="S10:S13"/>
+    <mergeCell ref="S14:S17"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="J1:K1"/>
@@ -4876,11 +4918,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="S6:S9"/>
-    <mergeCell ref="S2:S5"/>
-    <mergeCell ref="S10:S13"/>
-    <mergeCell ref="S14:S17"/>
   </mergeCells>
   <conditionalFormatting sqref="M3">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -4913,7 +4950,7 @@
   <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4922,80 +4959,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="42" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="53" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f>transaksi!M3</f>
-        <v>69000</v>
+        <v>89000</v>
       </c>
       <c r="B3" s="24">
-        <f>86000</f>
-        <v>86000</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+        <f>58000</f>
+        <v>58000</v>
+      </c>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45">
+      <c r="A4" s="60">
         <f>B3+A3</f>
-        <v>155000</v>
-      </c>
-      <c r="B4" s="41"/>
+        <v>147000</v>
+      </c>
+      <c r="B4" s="52"/>
       <c r="C4" s="12">
         <v>0</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12">
-        <v>112000</v>
+        <v>162000</v>
       </c>
       <c r="F4" s="12">
-        <v>121930</v>
+        <v>83290</v>
       </c>
       <c r="G4" s="13">
         <f>SUM($A$4:$F$4)</f>
-        <v>388930</v>
+        <v>392290</v>
       </c>
       <c r="H4" s="14">
         <f>G4-$A$3</f>
-        <v>319930</v>
+        <v>303290</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5268,14 +5305,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
@@ -5473,10 +5510,10 @@
       <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="41"/>
+      <c r="G1" s="52"/>
       <c r="H1" s="7" t="s">
         <v>79</v>
       </c>
@@ -5619,10 +5656,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="41"/>
+      <c r="G7" s="52"/>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
@@ -5638,7 +5675,7 @@
       </c>
       <c r="G8" s="23">
         <f>(transaksi!$K$3)*(H2/100)</f>
-        <v>58159.6875</v>
+        <v>60994.6875</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>81</v>
@@ -5658,7 +5695,7 @@
       </c>
       <c r="G9" s="23">
         <f>(transaksi!$K$3)*(H3/100)</f>
-        <v>10770.3125</v>
+        <v>11295.3125</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>